<commit_message>
manage all engine values with python
</commit_message>
<xml_diff>
--- a/REB Engine Profile.xlsx
+++ b/REB Engine Profile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgkid\Documents\GitHub\REBalanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5F1A6E-E7A9-48B3-B41A-00A34EFCF8A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2E0BC42-47AC-402E-A963-2B51E738B6B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{48F6B32E-432E-46EB-935F-18F86645025F}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="87">
   <si>
     <t>thrust</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -332,9 +332,6 @@
   <si>
     <t>F414-GE-400</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>F-16A/B</t>
   </si>
   <si>
     <t>F-16C/D Blk 50</t>
@@ -8132,7 +8129,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9305925" cy="6076950"/>
+    <xdr:ext cx="9298983" cy="6078242"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="차트 1">
@@ -8461,7 +8458,7 @@
   <dimension ref="A1:Z32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -8892,7 +8889,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="I6" s="3"/>
+      <c r="I6" s="2"/>
       <c r="J6" s="3"/>
       <c r="K6" s="2"/>
       <c r="L6" s="4"/>
@@ -8901,16 +8898,16 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>77</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" s="2">
-        <v>7390</v>
+        <v>8573</v>
       </c>
       <c r="E7" s="2">
         <v>3200</v>
@@ -8919,87 +8916,87 @@
         <v>12020</v>
       </c>
       <c r="G7" s="2">
-        <v>14670</v>
+        <v>16600</v>
       </c>
       <c r="H7" s="2">
-        <v>23830</v>
-      </c>
-      <c r="I7" s="6">
-        <v>0.73499999999999999</v>
+        <v>28000</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0.745</v>
       </c>
       <c r="J7" s="3">
-        <v>2.1</v>
+        <v>1.9710000000000001</v>
       </c>
       <c r="K7" s="2">
-        <v>228</v>
+        <v>264</v>
       </c>
       <c r="L7" s="4">
-        <f t="shared" ref="L7:M11" si="4">G7/224.809</f>
-        <v>65.255394579398512</v>
+        <f t="shared" ref="L6:M10" si="4">G7/224.809</f>
+        <v>73.840460123927429</v>
       </c>
       <c r="M7" s="4">
         <f t="shared" si="4"/>
-        <v>106.00109426224039</v>
+        <v>124.55017370301012</v>
       </c>
       <c r="N7" s="4">
-        <f t="shared" ref="N7:O11" si="5">I7*28.325</f>
-        <v>20.818874999999998</v>
+        <f t="shared" ref="N6:O10" si="5">I7*28.325</f>
+        <v>21.102125000000001</v>
       </c>
       <c r="O7" s="4">
         <f t="shared" si="5"/>
-        <v>59.482500000000002</v>
+        <v>55.828575000000001</v>
       </c>
       <c r="P7" s="5">
-        <f t="shared" ref="P7:Q11" si="6">L7*N7/1000</f>
-        <v>1.358543902824175</v>
+        <f t="shared" ref="P6:Q10" si="6">L7*N7/1000</f>
+        <v>1.5581906195926323</v>
       </c>
       <c r="Q7" s="5">
         <f t="shared" si="6"/>
-        <v>6.3052100894537144</v>
+        <v>6.9534587138415285</v>
       </c>
       <c r="R7" s="5">
         <f>K7/2.205</f>
-        <v>103.40136054421768</v>
+        <v>119.72789115646258</v>
       </c>
       <c r="S7" s="5">
         <f>(C7*L7*1000/9.81)/D7</f>
-        <v>0.90012531163001641</v>
+        <v>0.87799605218060006</v>
       </c>
       <c r="T7" s="5">
         <f>(C7*L7*1000/9.81)/F7</f>
-        <v>0.55340482969599181</v>
+        <v>0.62621132739969088</v>
       </c>
       <c r="U7" s="5">
         <f>(C7*M7*1000/9.81)/D7</f>
-        <v>1.4621667468400332</v>
+        <v>1.4809571964492048</v>
       </c>
       <c r="V7" s="5">
         <f>(C7*M7*1000/9.81)/F7</f>
-        <v>0.89895276698401383</v>
+        <v>1.0562600703127314</v>
       </c>
       <c r="W7" s="5">
         <f>E7/(P7*C7)</f>
-        <v>2355.4630758327057</v>
+        <v>2053.6640124534933</v>
       </c>
       <c r="X7" s="5">
         <f>E7/(Q7*C7)</f>
-        <v>507.51679239878416</v>
+        <v>460.20263176799943</v>
       </c>
       <c r="Y7" s="5">
-        <f t="shared" ref="Y7:Y8" si="7">W7*0.33</f>
-        <v>777.30281502479295</v>
+        <f t="shared" ref="Y6:Y7" si="7">W7*0.33</f>
+        <v>677.70912410965286</v>
       </c>
       <c r="Z7" s="5">
         <f>Q7/P7</f>
-        <v>4.641152984711268</v>
+        <v>4.462521225842969</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>77</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -9014,27 +9011,27 @@
         <v>12020</v>
       </c>
       <c r="G8" s="2">
-        <v>16600</v>
+        <v>17000</v>
       </c>
       <c r="H8" s="2">
-        <v>28000</v>
-      </c>
-      <c r="I8" s="3">
+        <v>29000</v>
+      </c>
+      <c r="I8" s="6">
         <v>0.745</v>
       </c>
       <c r="J8" s="3">
-        <v>1.9710000000000001</v>
+        <v>1.9</v>
       </c>
       <c r="K8" s="2">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="L8" s="4">
         <f t="shared" si="4"/>
-        <v>73.840460123927429</v>
+        <v>75.619748319684717</v>
       </c>
       <c r="M8" s="4">
         <f t="shared" si="4"/>
-        <v>124.55017370301012</v>
+        <v>128.99839419240334</v>
       </c>
       <c r="N8" s="4">
         <f t="shared" si="5"/>
@@ -9042,59 +9039,59 @@
       </c>
       <c r="O8" s="4">
         <f t="shared" si="5"/>
-        <v>55.828575000000001</v>
+        <v>53.817499999999995</v>
       </c>
       <c r="P8" s="5">
         <f t="shared" si="6"/>
-        <v>1.5581906195926323</v>
+        <v>1.5957373815105271</v>
       </c>
       <c r="Q8" s="5">
         <f t="shared" si="6"/>
-        <v>6.9534587138415285</v>
+        <v>6.942371079449666</v>
       </c>
       <c r="R8" s="5">
         <f>K8/2.205</f>
-        <v>119.72789115646258</v>
+        <v>122.44897959183673</v>
       </c>
       <c r="S8" s="5">
         <f>(C8*L8*1000/9.81)/D8</f>
-        <v>0.87799605218060006</v>
+        <v>0.89915258355844574</v>
       </c>
       <c r="T8" s="5">
         <f>(C8*L8*1000/9.81)/F8</f>
-        <v>0.62621132739969088</v>
+        <v>0.64130075697558697</v>
       </c>
       <c r="U8" s="5">
         <f>(C8*M8*1000/9.81)/D8</f>
-        <v>1.4809571964492048</v>
+        <v>1.5338485248938192</v>
       </c>
       <c r="V8" s="5">
         <f>(C8*M8*1000/9.81)/F8</f>
-        <v>1.0562600703127314</v>
+        <v>1.093983644252472</v>
       </c>
       <c r="W8" s="5">
         <f>E8/(P8*C8)</f>
-        <v>2053.6640124534933</v>
+        <v>2005.3425062781168</v>
       </c>
       <c r="X8" s="5">
         <f>E8/(Q8*C8)</f>
-        <v>460.20263176799943</v>
+        <v>460.93761963724785</v>
       </c>
       <c r="Y8" s="5">
-        <f t="shared" si="7"/>
-        <v>677.70912410965286</v>
+        <f>W8*0.33</f>
+        <v>661.76302707177854</v>
       </c>
       <c r="Z8" s="5">
         <f>Q8/P8</f>
-        <v>4.462521225842969</v>
+        <v>4.3505724437425961</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
         <v>78</v>
-      </c>
-      <c r="B9" t="s">
-        <v>21</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -9109,87 +9106,87 @@
         <v>12020</v>
       </c>
       <c r="G9" s="2">
-        <v>17000</v>
+        <v>14670</v>
       </c>
       <c r="H9" s="2">
-        <v>29000</v>
+        <v>23830</v>
       </c>
       <c r="I9" s="6">
-        <v>0.745</v>
+        <v>0.73499999999999999</v>
       </c>
       <c r="J9" s="3">
-        <v>1.9</v>
+        <v>2.1</v>
       </c>
       <c r="K9" s="2">
-        <v>270</v>
+        <v>228</v>
       </c>
       <c r="L9" s="4">
         <f t="shared" si="4"/>
-        <v>75.619748319684717</v>
+        <v>65.255394579398512</v>
       </c>
       <c r="M9" s="4">
         <f t="shared" si="4"/>
-        <v>128.99839419240334</v>
+        <v>106.00109426224039</v>
       </c>
       <c r="N9" s="4">
         <f t="shared" si="5"/>
-        <v>21.102125000000001</v>
+        <v>20.818874999999998</v>
       </c>
       <c r="O9" s="4">
         <f t="shared" si="5"/>
-        <v>53.817499999999995</v>
+        <v>59.482500000000002</v>
       </c>
       <c r="P9" s="5">
         <f t="shared" si="6"/>
-        <v>1.5957373815105271</v>
+        <v>1.358543902824175</v>
       </c>
       <c r="Q9" s="5">
         <f t="shared" si="6"/>
-        <v>6.942371079449666</v>
+        <v>6.3052100894537144</v>
       </c>
       <c r="R9" s="5">
         <f>K9/2.205</f>
-        <v>122.44897959183673</v>
+        <v>103.40136054421768</v>
       </c>
       <c r="S9" s="5">
         <f>(C9*L9*1000/9.81)/D9</f>
-        <v>0.89915258355844574</v>
+        <v>0.77591578828249408</v>
       </c>
       <c r="T9" s="5">
         <f>(C9*L9*1000/9.81)/F9</f>
-        <v>0.64130075697558697</v>
+        <v>0.55340482969599181</v>
       </c>
       <c r="U9" s="5">
         <f>(C9*M9*1000/9.81)/D9</f>
-        <v>1.5338485248938192</v>
+        <v>1.2604003568351623</v>
       </c>
       <c r="V9" s="5">
         <f>(C9*M9*1000/9.81)/F9</f>
-        <v>1.093983644252472</v>
+        <v>0.89895276698401383</v>
       </c>
       <c r="W9" s="5">
         <f>E9/(P9*C9)</f>
-        <v>2005.3425062781168</v>
+        <v>2355.4630758327057</v>
       </c>
       <c r="X9" s="5">
         <f>E9/(Q9*C9)</f>
-        <v>460.93761963724785</v>
+        <v>507.51679239878416</v>
       </c>
       <c r="Y9" s="5">
         <f>W9*0.33</f>
-        <v>661.76302707177854</v>
+        <v>777.30281502479295</v>
       </c>
       <c r="Z9" s="5">
         <f>Q9/P9</f>
-        <v>4.3505724437425961</v>
+        <v>4.641152984711268</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>79</v>
       </c>
       <c r="B10" t="s">
-        <v>79</v>
+        <v>22</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -9204,202 +9201,202 @@
         <v>12020</v>
       </c>
       <c r="G10" s="2">
-        <v>14670</v>
+        <v>17800</v>
       </c>
       <c r="H10" s="2">
-        <v>23830</v>
-      </c>
-      <c r="I10" s="6">
-        <v>0.73499999999999999</v>
+        <v>29100</v>
+      </c>
+      <c r="I10" s="3">
+        <v>0.72599999999999998</v>
       </c>
       <c r="J10" s="3">
-        <v>2.1</v>
+        <v>2.06</v>
       </c>
       <c r="K10" s="2">
-        <v>228</v>
+        <v>254</v>
       </c>
       <c r="L10" s="4">
         <f t="shared" si="4"/>
-        <v>65.255394579398512</v>
+        <v>79.178324711199281</v>
       </c>
       <c r="M10" s="4">
         <f t="shared" si="4"/>
-        <v>106.00109426224039</v>
+        <v>129.44321624134264</v>
       </c>
       <c r="N10" s="4">
         <f t="shared" si="5"/>
-        <v>20.818874999999998</v>
+        <v>20.563949999999998</v>
       </c>
       <c r="O10" s="4">
         <f t="shared" si="5"/>
-        <v>59.482500000000002</v>
+        <v>58.349499999999999</v>
       </c>
       <c r="P10" s="5">
         <f t="shared" si="6"/>
-        <v>1.358543902824175</v>
+        <v>1.6282191104448664</v>
       </c>
       <c r="Q10" s="5">
         <f t="shared" si="6"/>
-        <v>6.3052100894537144</v>
+        <v>7.552946946074222</v>
       </c>
       <c r="R10" s="5">
         <f>K10/2.205</f>
-        <v>103.40136054421768</v>
+        <v>115.19274376417233</v>
       </c>
       <c r="S10" s="5">
         <f>(C10*L10*1000/9.81)/D10</f>
-        <v>0.77591578828249408</v>
+        <v>0.94146564631413721</v>
       </c>
       <c r="T10" s="5">
         <f>(C10*L10*1000/9.81)/F10</f>
-        <v>0.55340482969599181</v>
+        <v>0.67147961612737928</v>
       </c>
       <c r="U10" s="5">
         <f>(C10*M10*1000/9.81)/D10</f>
-        <v>1.2604003568351623</v>
+        <v>1.5391376577382805</v>
       </c>
       <c r="V10" s="5">
         <f>(C10*M10*1000/9.81)/F10</f>
-        <v>0.89895276698401383</v>
+        <v>1.0977560016464458</v>
       </c>
       <c r="W10" s="5">
         <f>E10/(P10*C10)</f>
-        <v>2355.4630758327057</v>
+        <v>1965.3374533392421</v>
       </c>
       <c r="X10" s="5">
         <f>E10/(Q10*C10)</f>
-        <v>507.51679239878416</v>
+        <v>423.6756888201441</v>
       </c>
       <c r="Y10" s="5">
         <f>W10*0.33</f>
-        <v>777.30281502479295</v>
+        <v>648.5613596019499</v>
       </c>
       <c r="Z10" s="5">
         <f>Q10/P10</f>
+        <v>4.638777973813724</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="Q11" s="5"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2">
+        <v>12701</v>
+      </c>
+      <c r="E12" s="2">
+        <v>6103</v>
+      </c>
+      <c r="F12" s="2">
+        <v>20185</v>
+      </c>
+      <c r="G12" s="2">
+        <v>14670</v>
+      </c>
+      <c r="H12" s="2">
+        <v>23830</v>
+      </c>
+      <c r="I12" s="6">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="J12" s="3">
+        <v>2.1</v>
+      </c>
+      <c r="K12" s="2">
+        <v>228</v>
+      </c>
+      <c r="L12" s="4">
+        <f t="shared" ref="L12:M15" si="8">G12/224.809</f>
+        <v>65.255394579398512</v>
+      </c>
+      <c r="M12" s="4">
+        <f t="shared" si="8"/>
+        <v>106.00109426224039</v>
+      </c>
+      <c r="N12" s="4">
+        <f t="shared" ref="N12:O15" si="9">I12*28.325</f>
+        <v>20.818874999999998</v>
+      </c>
+      <c r="O12" s="4">
+        <f t="shared" si="9"/>
+        <v>59.482500000000002</v>
+      </c>
+      <c r="P12" s="5">
+        <f t="shared" ref="P12:Q15" si="10">L12*N12/1000</f>
+        <v>1.358543902824175</v>
+      </c>
+      <c r="Q12" s="5">
+        <f t="shared" si="10"/>
+        <v>6.3052100894537144</v>
+      </c>
+      <c r="R12" s="5">
+        <f>K12/2.205</f>
+        <v>103.40136054421768</v>
+      </c>
+      <c r="S12" s="5">
+        <f>(C12*L12*1000/9.81)/D12</f>
+        <v>1.0474649323589988</v>
+      </c>
+      <c r="T12" s="5">
+        <f>(C12*L12*1000/9.81)/F12</f>
+        <v>0.65909596759433453</v>
+      </c>
+      <c r="U12" s="5">
+        <f>(C12*M12*1000/9.81)/D12</f>
+        <v>1.701505749019423</v>
+      </c>
+      <c r="V12" s="5">
+        <f>(C12*M12*1000/9.81)/F12</f>
+        <v>1.0706378260240621</v>
+      </c>
+      <c r="W12" s="5">
+        <f>E12/(P12*C12)</f>
+        <v>2246.1548674698442</v>
+      </c>
+      <c r="X12" s="5">
+        <f>E12/(Q12*C12)</f>
+        <v>483.96484125152807</v>
+      </c>
+      <c r="Y12" s="5">
+        <f>W12*0.33</f>
+        <v>741.23110626504865</v>
+      </c>
+      <c r="Z12" s="5">
+        <f>Q12/P12</f>
         <v>4.641152984711268</v>
       </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>80</v>
-      </c>
-      <c r="B11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" s="2">
-        <v>8573</v>
-      </c>
-      <c r="E11" s="2">
-        <v>3200</v>
-      </c>
-      <c r="F11" s="2">
-        <v>12020</v>
-      </c>
-      <c r="G11" s="2">
-        <v>17800</v>
-      </c>
-      <c r="H11" s="2">
-        <v>29100</v>
-      </c>
-      <c r="I11" s="3">
-        <v>0.72599999999999998</v>
-      </c>
-      <c r="J11" s="3">
-        <v>2.06</v>
-      </c>
-      <c r="K11" s="2">
-        <v>254</v>
-      </c>
-      <c r="L11" s="4">
-        <f t="shared" si="4"/>
-        <v>79.178324711199281</v>
-      </c>
-      <c r="M11" s="4">
-        <f t="shared" si="4"/>
-        <v>129.44321624134264</v>
-      </c>
-      <c r="N11" s="4">
-        <f t="shared" si="5"/>
-        <v>20.563949999999998</v>
-      </c>
-      <c r="O11" s="4">
-        <f t="shared" si="5"/>
-        <v>58.349499999999999</v>
-      </c>
-      <c r="P11" s="5">
-        <f t="shared" si="6"/>
-        <v>1.6282191104448664</v>
-      </c>
-      <c r="Q11" s="5">
-        <f t="shared" si="6"/>
-        <v>7.552946946074222</v>
-      </c>
-      <c r="R11" s="5">
-        <f>K11/2.205</f>
-        <v>115.19274376417233</v>
-      </c>
-      <c r="S11" s="5">
-        <f>(C11*L11*1000/9.81)/D11</f>
-        <v>0.94146564631413721</v>
-      </c>
-      <c r="T11" s="5">
-        <f>(C11*L11*1000/9.81)/F11</f>
-        <v>0.67147961612737928</v>
-      </c>
-      <c r="U11" s="5">
-        <f>(C11*M11*1000/9.81)/D11</f>
-        <v>1.5391376577382805</v>
-      </c>
-      <c r="V11" s="5">
-        <f>(C11*M11*1000/9.81)/F11</f>
-        <v>1.0977560016464458</v>
-      </c>
-      <c r="W11" s="5">
-        <f>E11/(P11*C11)</f>
-        <v>1965.3374533392421</v>
-      </c>
-      <c r="X11" s="5">
-        <f>E11/(Q11*C11)</f>
-        <v>423.6756888201441</v>
-      </c>
-      <c r="Y11" s="5">
-        <f>W11*0.33</f>
-        <v>648.5613596019499</v>
-      </c>
-      <c r="Z11" s="5">
-        <f>Q11/P11</f>
-        <v>4.638777973813724</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="Q12" s="5"/>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>81</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>78</v>
       </c>
       <c r="C13">
         <v>2</v>
       </c>
       <c r="D13" s="2">
-        <v>12701</v>
+        <v>14379</v>
       </c>
       <c r="E13" s="2">
-        <v>6103</v>
+        <v>10591</v>
       </c>
       <c r="F13" s="2">
-        <v>20185</v>
+        <v>23000</v>
       </c>
       <c r="G13" s="2">
         <v>14670</v>
@@ -9417,7 +9414,7 @@
         <v>228</v>
       </c>
       <c r="L13" s="4">
-        <f t="shared" ref="L13:M16" si="8">G13/224.809</f>
+        <f t="shared" si="8"/>
         <v>65.255394579398512</v>
       </c>
       <c r="M13" s="4">
@@ -9425,7 +9422,7 @@
         <v>106.00109426224039</v>
       </c>
       <c r="N13" s="4">
-        <f t="shared" ref="N13:O16" si="9">I13*28.325</f>
+        <f t="shared" si="9"/>
         <v>20.818874999999998</v>
       </c>
       <c r="O13" s="4">
@@ -9433,7 +9430,7 @@
         <v>59.482500000000002</v>
       </c>
       <c r="P13" s="5">
-        <f t="shared" ref="P13:Q16" si="10">L13*N13/1000</f>
+        <f t="shared" si="10"/>
         <v>1.358543902824175</v>
       </c>
       <c r="Q13" s="5">
@@ -9446,31 +9443,31 @@
       </c>
       <c r="S13" s="5">
         <f>(C13*L13*1000/9.81)/D13</f>
-        <v>1.0474649323589988</v>
+        <v>0.92522790916556386</v>
       </c>
       <c r="T13" s="5">
         <f>(C13*L13*1000/9.81)/F13</f>
-        <v>0.65909596759433453</v>
+        <v>0.5784283524300714</v>
       </c>
       <c r="U13" s="5">
         <f>(C13*M13*1000/9.81)/D13</f>
-        <v>1.701505749019423</v>
+        <v>1.5029434952566725</v>
       </c>
       <c r="V13" s="5">
         <f>(C13*M13*1000/9.81)/F13</f>
-        <v>1.0706378260240621</v>
+        <v>0.9396010660128562</v>
       </c>
       <c r="W13" s="5">
         <f>E13/(P13*C13)</f>
-        <v>2246.1548674698442</v>
+        <v>3897.9233493975294</v>
       </c>
       <c r="X13" s="5">
         <f>E13/(Q13*C13)</f>
-        <v>483.96484125152807</v>
+        <v>839.86099192117547</v>
       </c>
       <c r="Y13" s="5">
         <f>W13*0.33</f>
-        <v>741.23110626504865</v>
+        <v>1286.3147053011849</v>
       </c>
       <c r="Z13" s="5">
         <f>Q13/P13</f>
@@ -9479,10 +9476,10 @@
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B14" t="s">
-        <v>79</v>
+        <v>21</v>
       </c>
       <c r="C14">
         <v>2</v>
@@ -9497,87 +9494,87 @@
         <v>23000</v>
       </c>
       <c r="G14" s="2">
-        <v>14670</v>
+        <v>17000</v>
       </c>
       <c r="H14" s="2">
-        <v>23830</v>
+        <v>28000</v>
       </c>
       <c r="I14" s="6">
-        <v>0.73499999999999999</v>
+        <v>0.745</v>
       </c>
       <c r="J14" s="3">
-        <v>2.1</v>
+        <v>1.9</v>
       </c>
       <c r="K14" s="2">
-        <v>228</v>
+        <v>270</v>
       </c>
       <c r="L14" s="4">
         <f t="shared" si="8"/>
-        <v>65.255394579398512</v>
+        <v>75.619748319684717</v>
       </c>
       <c r="M14" s="4">
         <f t="shared" si="8"/>
-        <v>106.00109426224039</v>
+        <v>124.55017370301012</v>
       </c>
       <c r="N14" s="4">
         <f t="shared" si="9"/>
-        <v>20.818874999999998</v>
+        <v>21.102125000000001</v>
       </c>
       <c r="O14" s="4">
         <f t="shared" si="9"/>
-        <v>59.482500000000002</v>
+        <v>53.817499999999995</v>
       </c>
       <c r="P14" s="5">
         <f t="shared" si="10"/>
-        <v>1.358543902824175</v>
+        <v>1.5957373815105271</v>
       </c>
       <c r="Q14" s="5">
         <f t="shared" si="10"/>
-        <v>6.3052100894537144</v>
+        <v>6.7029789732617466</v>
       </c>
       <c r="R14" s="5">
         <f>K14/2.205</f>
-        <v>103.40136054421768</v>
+        <v>122.44897959183673</v>
       </c>
       <c r="S14" s="5">
         <f>(C14*L14*1000/9.81)/D14</f>
-        <v>0.92522790916556386</v>
+        <v>1.0721795811734551</v>
       </c>
       <c r="T14" s="5">
         <f>(C14*L14*1000/9.81)/F14</f>
-        <v>0.5784283524300714</v>
+        <v>0.67029870424752658</v>
       </c>
       <c r="U14" s="5">
         <f>(C14*M14*1000/9.81)/D14</f>
-        <v>1.5029434952566725</v>
+        <v>1.7659428395798085</v>
       </c>
       <c r="V14" s="5">
         <f>(C14*M14*1000/9.81)/F14</f>
-        <v>0.9396010660128562</v>
+        <v>1.1040213952312201</v>
       </c>
       <c r="W14" s="5">
         <f>E14/(P14*C14)</f>
-        <v>3897.9233493975294</v>
+        <v>3318.5285131236774</v>
       </c>
       <c r="X14" s="5">
         <f>E14/(Q14*C14)</f>
-        <v>839.86099192117547</v>
+        <v>790.02187253216891</v>
       </c>
       <c r="Y14" s="5">
         <f>W14*0.33</f>
-        <v>1286.3147053011849</v>
+        <v>1095.1144093308135</v>
       </c>
       <c r="Z14" s="5">
         <f>Q14/P14</f>
-        <v>4.641152984711268</v>
+        <v>4.2005527043031963</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C15">
         <v>2</v>
@@ -9592,190 +9589,190 @@
         <v>23000</v>
       </c>
       <c r="G15" s="2">
-        <v>17000</v>
+        <v>17800</v>
       </c>
       <c r="H15" s="2">
-        <v>28000</v>
-      </c>
-      <c r="I15" s="6">
-        <v>0.745</v>
+        <v>29100</v>
+      </c>
+      <c r="I15" s="3">
+        <v>0.72599999999999998</v>
       </c>
       <c r="J15" s="3">
-        <v>1.9</v>
+        <v>2.06</v>
       </c>
       <c r="K15" s="2">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="L15" s="4">
         <f t="shared" si="8"/>
-        <v>75.619748319684717</v>
+        <v>79.178324711199281</v>
       </c>
       <c r="M15" s="4">
         <f t="shared" si="8"/>
-        <v>124.55017370301012</v>
+        <v>129.44321624134264</v>
       </c>
       <c r="N15" s="4">
         <f t="shared" si="9"/>
-        <v>21.102125000000001</v>
+        <v>20.563949999999998</v>
       </c>
       <c r="O15" s="4">
         <f t="shared" si="9"/>
-        <v>53.817499999999995</v>
+        <v>58.349499999999999</v>
       </c>
       <c r="P15" s="5">
         <f t="shared" si="10"/>
-        <v>1.5957373815105271</v>
+        <v>1.6282191104448664</v>
       </c>
       <c r="Q15" s="5">
         <f t="shared" si="10"/>
-        <v>6.7029789732617466</v>
+        <v>7.552946946074222</v>
       </c>
       <c r="R15" s="5">
         <f>K15/2.205</f>
-        <v>122.44897959183673</v>
+        <v>115.19274376417233</v>
       </c>
       <c r="S15" s="5">
         <f>(C15*L15*1000/9.81)/D15</f>
-        <v>1.0721795811734551</v>
+        <v>1.1226350908757352</v>
       </c>
       <c r="T15" s="5">
         <f>(C15*L15*1000/9.81)/F15</f>
-        <v>0.67029870424752658</v>
+        <v>0.70184217268270421</v>
       </c>
       <c r="U15" s="5">
         <f>(C15*M15*1000/9.81)/D15</f>
-        <v>1.7659428395798085</v>
+        <v>1.8353191654204435</v>
       </c>
       <c r="V15" s="5">
         <f>(C15*M15*1000/9.81)/F15</f>
-        <v>1.1040213952312201</v>
+        <v>1.1473936643295894</v>
       </c>
       <c r="W15" s="5">
         <f>E15/(P15*C15)</f>
-        <v>3318.5285131236774</v>
+        <v>3252.3264012993614</v>
       </c>
       <c r="X15" s="5">
         <f>E15/(Q15*C15)</f>
-        <v>790.02187253216891</v>
+        <v>701.11706567096041</v>
       </c>
       <c r="Y15" s="5">
         <f>W15*0.33</f>
-        <v>1095.1144093308135</v>
+        <v>1073.2677124287893</v>
       </c>
       <c r="Z15" s="5">
         <f>Q15/P15</f>
-        <v>4.2005527043031963</v>
+        <v>4.638777973813724</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>82</v>
-      </c>
-      <c r="B16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16">
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="Q16" s="5"/>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17">
         <v>2</v>
       </c>
-      <c r="D16" s="2">
-        <v>14379</v>
-      </c>
-      <c r="E16" s="2">
-        <v>10591</v>
-      </c>
-      <c r="F16" s="2">
-        <v>23000</v>
-      </c>
-      <c r="G16" s="2">
-        <v>17800</v>
-      </c>
-      <c r="H16" s="2">
-        <v>29100</v>
-      </c>
-      <c r="I16" s="3">
-        <v>0.72599999999999998</v>
-      </c>
-      <c r="J16" s="3">
-        <v>2.06</v>
-      </c>
-      <c r="K16" s="2">
-        <v>254</v>
-      </c>
-      <c r="L16" s="4">
-        <f t="shared" si="8"/>
-        <v>79.178324711199281</v>
-      </c>
-      <c r="M16" s="4">
-        <f t="shared" si="8"/>
-        <v>129.44321624134264</v>
-      </c>
-      <c r="N16" s="4">
-        <f t="shared" si="9"/>
-        <v>20.563949999999998</v>
-      </c>
-      <c r="O16" s="4">
-        <f t="shared" si="9"/>
-        <v>58.349499999999999</v>
-      </c>
-      <c r="P16" s="5">
-        <f t="shared" si="10"/>
-        <v>1.6282191104448664</v>
-      </c>
-      <c r="Q16" s="5">
-        <f t="shared" si="10"/>
-        <v>7.552946946074222</v>
-      </c>
-      <c r="R16" s="5">
-        <f>K16/2.205</f>
-        <v>115.19274376417233</v>
-      </c>
-      <c r="S16" s="5">
-        <f>(C16*L16*1000/9.81)/D16</f>
-        <v>1.1226350908757352</v>
-      </c>
-      <c r="T16" s="5">
-        <f>(C16*L16*1000/9.81)/F16</f>
-        <v>0.70184217268270421</v>
-      </c>
-      <c r="U16" s="5">
-        <f>(C16*M16*1000/9.81)/D16</f>
-        <v>1.8353191654204435</v>
-      </c>
-      <c r="V16" s="5">
-        <f>(C16*M16*1000/9.81)/F16</f>
-        <v>1.1473936643295894</v>
-      </c>
-      <c r="W16" s="5">
-        <f>E16/(P16*C16)</f>
-        <v>3252.3264012993614</v>
-      </c>
-      <c r="X16" s="5">
-        <f>E16/(Q16*C16)</f>
-        <v>701.11706567096041</v>
-      </c>
-      <c r="Y16" s="5">
-        <f>W16*0.33</f>
-        <v>1073.2677124287893</v>
-      </c>
-      <c r="Z16" s="5">
-        <f>Q16/P16</f>
-        <v>4.638777973813724</v>
-      </c>
-    </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="4"/>
-      <c r="O17" s="4"/>
-      <c r="Q17" s="5"/>
+      <c r="D17" s="2">
+        <v>19838</v>
+      </c>
+      <c r="E17" s="2">
+        <v>7350</v>
+      </c>
+      <c r="F17" s="2">
+        <v>27669</v>
+      </c>
+      <c r="G17" s="7">
+        <v>12350</v>
+      </c>
+      <c r="H17" s="2">
+        <v>20900</v>
+      </c>
+      <c r="I17" s="6">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="J17" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="K17" s="7">
+        <v>260</v>
+      </c>
+      <c r="L17" s="4">
+        <f>G17/224.809</f>
+        <v>54.935523044006246</v>
+      </c>
+      <c r="M17" s="4">
+        <f>H17/224.809</f>
+        <v>92.967808228318262</v>
+      </c>
+      <c r="N17" s="4">
+        <f>I17*28.325</f>
+        <v>18.892775</v>
+      </c>
+      <c r="O17" s="4">
+        <f>J17*28.325</f>
+        <v>70.8125</v>
+      </c>
+      <c r="P17" s="5">
+        <f>L17*N17/1000</f>
+        <v>1.0378844763777251</v>
+      </c>
+      <c r="Q17" s="5">
+        <f>M17*O17/1000</f>
+        <v>6.5832829201677869</v>
+      </c>
+      <c r="R17" s="5">
+        <f>K17/2.205</f>
+        <v>117.91383219954648</v>
+      </c>
+      <c r="S17" s="5">
+        <f>(C17*L17*1000/9.81)/D17</f>
+        <v>0.56456813999724209</v>
+      </c>
+      <c r="T17" s="5">
+        <f>(C17*L17*1000/9.81)/F17</f>
+        <v>0.40478162424609809</v>
+      </c>
+      <c r="U17" s="5">
+        <f>(C17*M17*1000/9.81)/D17</f>
+        <v>0.95542300614917886</v>
+      </c>
+      <c r="V17" s="5">
+        <f>(C17*M17*1000/9.81)/F17</f>
+        <v>0.68501505641647376</v>
+      </c>
+      <c r="W17" s="5">
+        <f>E17/(P17*C17)</f>
+        <v>3540.8565053655643</v>
+      </c>
+      <c r="X17" s="5">
+        <f>E17/(Q17*C17)</f>
+        <v>558.23212287317824</v>
+      </c>
+      <c r="Y17" s="5">
+        <f t="shared" ref="Y17:Y18" si="11">W17*0.33</f>
+        <v>1168.4826467706364</v>
+      </c>
+      <c r="Z17" s="5">
+        <f>Q17/P17</f>
+        <v>6.3429823549763578</v>
+      </c>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="C18">
         <v>2</v>
@@ -9789,263 +9786,232 @@
       <c r="F18" s="2">
         <v>27669</v>
       </c>
-      <c r="G18" s="7">
-        <v>12350</v>
+      <c r="G18" s="2">
+        <v>16800</v>
       </c>
       <c r="H18" s="2">
-        <v>20900</v>
+        <v>26080</v>
       </c>
       <c r="I18" s="6">
-        <v>0.66700000000000004</v>
-      </c>
-      <c r="J18" s="6">
-        <v>2.5</v>
-      </c>
-      <c r="K18" s="7">
-        <v>260</v>
+        <v>0.745</v>
+      </c>
+      <c r="J18" s="3">
+        <v>2</v>
+      </c>
+      <c r="K18" s="2">
+        <v>250</v>
       </c>
       <c r="L18" s="4">
         <f>G18/224.809</f>
-        <v>54.935523044006246</v>
+        <v>74.730104221806073</v>
       </c>
       <c r="M18" s="4">
         <f>H18/224.809</f>
-        <v>92.967808228318262</v>
+        <v>116.00959036337514</v>
       </c>
       <c r="N18" s="4">
         <f>I18*28.325</f>
-        <v>18.892775</v>
+        <v>21.102125000000001</v>
       </c>
       <c r="O18" s="4">
         <f>J18*28.325</f>
-        <v>70.8125</v>
+        <v>56.65</v>
       </c>
       <c r="P18" s="5">
         <f>L18*N18/1000</f>
-        <v>1.0378844763777251</v>
+        <v>1.5769640005515797</v>
       </c>
       <c r="Q18" s="5">
         <f>M18*O18/1000</f>
-        <v>6.5832829201677869</v>
+        <v>6.5719432940852007</v>
       </c>
       <c r="R18" s="5">
         <f>K18/2.205</f>
-        <v>117.91383219954648</v>
+        <v>113.37868480725623</v>
       </c>
       <c r="S18" s="5">
         <f>(C18*L18*1000/9.81)/D18</f>
-        <v>0.56456813999724209</v>
+        <v>0.76799552647398128</v>
       </c>
       <c r="T18" s="5">
         <f>(C18*L18*1000/9.81)/F18</f>
-        <v>0.40478162424609809</v>
+        <v>0.55063411233477322</v>
       </c>
       <c r="U18" s="5">
         <f>(C18*M18*1000/9.81)/D18</f>
-        <v>0.95542300614917886</v>
+        <v>1.1922216268119898</v>
       </c>
       <c r="V18" s="5">
         <f>(C18*M18*1000/9.81)/F18</f>
-        <v>0.68501505641647376</v>
+        <v>0.85479390771969554</v>
       </c>
       <c r="W18" s="5">
         <f>E18/(P18*C18)</f>
-        <v>3540.8565053655643</v>
+        <v>2330.4273266317959</v>
       </c>
       <c r="X18" s="5">
         <f>E18/(Q18*C18)</f>
-        <v>558.23212287317824</v>
+        <v>559.19533014040587</v>
       </c>
       <c r="Y18" s="5">
-        <f t="shared" ref="Y18:Y19" si="11">W18*0.33</f>
-        <v>1168.4826467706364</v>
+        <f t="shared" si="11"/>
+        <v>769.0410177884927</v>
       </c>
       <c r="Z18" s="5">
         <f>Q18/P18</f>
-        <v>6.3429823549763578</v>
+        <v>4.1674656439757101</v>
       </c>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19">
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="Q19" s="5"/>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20">
         <v>2</v>
       </c>
-      <c r="D19" s="2">
-        <v>19838</v>
-      </c>
-      <c r="E19" s="2">
-        <v>7350</v>
-      </c>
-      <c r="F19" s="2">
-        <v>27669</v>
-      </c>
-      <c r="G19" s="2">
-        <v>16800</v>
-      </c>
-      <c r="H19" s="2">
-        <v>26080</v>
-      </c>
-      <c r="I19" s="6">
-        <v>0.745</v>
-      </c>
-      <c r="J19" s="3">
-        <v>2</v>
-      </c>
-      <c r="K19" s="2">
-        <v>250</v>
-      </c>
-      <c r="L19" s="4">
-        <f>G19/224.809</f>
-        <v>74.730104221806073</v>
-      </c>
-      <c r="M19" s="4">
-        <f>H19/224.809</f>
-        <v>116.00959036337514</v>
-      </c>
-      <c r="N19" s="4">
-        <f>I19*28.325</f>
-        <v>21.102125000000001</v>
-      </c>
-      <c r="O19" s="4">
-        <f>J19*28.325</f>
-        <v>56.65</v>
-      </c>
-      <c r="P19" s="5">
-        <f>L19*N19/1000</f>
-        <v>1.5769640005515797</v>
-      </c>
-      <c r="Q19" s="5">
-        <f>M19*O19/1000</f>
-        <v>6.5719432940852007</v>
-      </c>
-      <c r="R19" s="5">
-        <f>K19/2.205</f>
-        <v>113.37868480725623</v>
-      </c>
-      <c r="S19" s="5">
-        <f>(C19*L19*1000/9.81)/D19</f>
-        <v>0.76799552647398128</v>
-      </c>
-      <c r="T19" s="5">
-        <f>(C19*L19*1000/9.81)/F19</f>
-        <v>0.55063411233477322</v>
-      </c>
-      <c r="U19" s="5">
-        <f>(C19*M19*1000/9.81)/D19</f>
-        <v>1.1922216268119898</v>
-      </c>
-      <c r="V19" s="5">
-        <f>(C19*M19*1000/9.81)/F19</f>
-        <v>0.85479390771969554</v>
-      </c>
-      <c r="W19" s="5">
-        <f>E19/(P19*C19)</f>
-        <v>2330.4273266317959</v>
-      </c>
-      <c r="X19" s="5">
-        <f>E19/(Q19*C19)</f>
-        <v>559.19533014040587</v>
-      </c>
-      <c r="Y19" s="5">
-        <f t="shared" si="11"/>
-        <v>769.0410177884927</v>
-      </c>
-      <c r="Z19" s="5">
-        <f>Q19/P19</f>
-        <v>4.1674656439757101</v>
-      </c>
-    </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="I20" s="3"/>
+      <c r="D20" s="2">
+        <v>11321</v>
+      </c>
+      <c r="E20" s="2">
+        <v>4990</v>
+      </c>
+      <c r="F20" s="2">
+        <v>13782</v>
+      </c>
+      <c r="G20" s="2">
+        <v>9065</v>
+      </c>
+      <c r="I20" s="6">
+        <v>0.37</v>
+      </c>
       <c r="J20" s="3"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="4"/>
+      <c r="K20" s="2">
+        <v>333</v>
+      </c>
+      <c r="L20" s="4">
+        <f>G20/224.809</f>
+        <v>40.323118736349521</v>
+      </c>
+      <c r="N20" s="4">
+        <f>I20*28.325</f>
+        <v>10.48025</v>
+      </c>
       <c r="O20" s="4"/>
+      <c r="P20" s="5">
+        <f>L20*N20/1000</f>
+        <v>0.42259636513662707</v>
+      </c>
       <c r="Q20" s="5"/>
+      <c r="R20" s="5">
+        <f>K20/2.205</f>
+        <v>151.0204081632653</v>
+      </c>
+      <c r="S20" s="5">
+        <f>(C20*L20*1000/9.81)/D20</f>
+        <v>0.7261566393640555</v>
+      </c>
+      <c r="T20" s="5">
+        <f>(C20*L20*1000/9.81)/F20</f>
+        <v>0.59648957438981809</v>
+      </c>
+      <c r="W20" s="5">
+        <f>E20/(P20*C20)</f>
+        <v>5903.9788456139622</v>
+      </c>
+      <c r="Y20" s="5">
+        <f t="shared" ref="Y20" si="12">W20*0.33</f>
+        <v>1948.3130190526076</v>
+      </c>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>83</v>
-      </c>
-      <c r="B21" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21">
-        <v>2</v>
-      </c>
-      <c r="D21" s="2">
-        <v>11321</v>
-      </c>
-      <c r="E21" s="2">
-        <v>4990</v>
-      </c>
-      <c r="F21" s="2">
-        <v>13782</v>
-      </c>
-      <c r="G21" s="2">
-        <v>9065</v>
-      </c>
-      <c r="I21" s="6">
-        <v>0.37</v>
-      </c>
+      <c r="I21" s="3"/>
       <c r="J21" s="3"/>
-      <c r="K21" s="2">
-        <v>333</v>
-      </c>
-      <c r="L21" s="4">
-        <f>G21/224.809</f>
-        <v>40.323118736349521</v>
-      </c>
-      <c r="N21" s="4">
-        <f>I21*28.325</f>
-        <v>10.48025</v>
-      </c>
+      <c r="K21" s="2"/>
+      <c r="L21" s="4"/>
       <c r="O21" s="4"/>
-      <c r="P21" s="5">
-        <f>L21*N21/1000</f>
-        <v>0.42259636513662707</v>
-      </c>
       <c r="Q21" s="5"/>
-      <c r="R21" s="5">
-        <f>K21/2.205</f>
-        <v>151.0204081632653</v>
-      </c>
-      <c r="S21" s="5">
-        <f>(C21*L21*1000/9.81)/D21</f>
-        <v>0.7261566393640555</v>
-      </c>
-      <c r="T21" s="5">
-        <f>(C21*L21*1000/9.81)/F21</f>
-        <v>0.59648957438981809</v>
-      </c>
-      <c r="W21" s="5">
-        <f>E21/(P21*C21)</f>
-        <v>5903.9788456139622</v>
-      </c>
-      <c r="Y21" s="5">
-        <f t="shared" ref="Y21" si="12">W21*0.33</f>
-        <v>1948.3130190526076</v>
-      </c>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="I22" s="3"/>
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" s="8">
+        <v>6340</v>
+      </c>
+      <c r="E22" s="8">
+        <v>3400</v>
+      </c>
+      <c r="F22" s="8">
+        <v>10410</v>
+      </c>
+      <c r="G22" s="2">
+        <v>21450</v>
+      </c>
+      <c r="I22" s="3">
+        <v>0.74</v>
+      </c>
       <c r="J22" s="3"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="4"/>
+      <c r="K22" s="7">
+        <v>459</v>
+      </c>
+      <c r="L22" s="4">
+        <f>G22/224.809</f>
+        <v>95.41432949748453</v>
+      </c>
+      <c r="N22" s="4">
+        <f>I22*28.325</f>
+        <v>20.9605</v>
+      </c>
       <c r="O22" s="4"/>
+      <c r="P22" s="5">
+        <f>L22*N22/1000</f>
+        <v>1.9999320534320246</v>
+      </c>
       <c r="Q22" s="5"/>
+      <c r="R22" s="5">
+        <f>K22/2.205</f>
+        <v>208.16326530612244</v>
+      </c>
+      <c r="S22" s="5">
+        <f>(C22*L22*1000/9.81)/D22</f>
+        <v>1.5341058904273392</v>
+      </c>
+      <c r="T22" s="5">
+        <f>(C22*L22*1000/9.81)/F22</f>
+        <v>0.93431617149945534</v>
+      </c>
+      <c r="W22" s="5">
+        <f>E22/(P22*C22)</f>
+        <v>1700.0577565449585</v>
+      </c>
+      <c r="Y22" s="5">
+        <f t="shared" ref="Y22:Y24" si="13">W22*0.33</f>
+        <v>561.01905965983633</v>
+      </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -10060,27 +10026,27 @@
         <v>10410</v>
       </c>
       <c r="G23" s="2">
-        <v>21450</v>
+        <v>23800</v>
       </c>
       <c r="I23" s="3">
-        <v>0.74</v>
+        <v>0.76</v>
       </c>
       <c r="J23" s="3"/>
-      <c r="K23" s="7">
+      <c r="K23" s="2">
         <v>459</v>
       </c>
       <c r="L23" s="4">
         <f>G23/224.809</f>
-        <v>95.41432949748453</v>
+        <v>105.8676476475586</v>
       </c>
       <c r="N23" s="4">
         <f>I23*28.325</f>
-        <v>20.9605</v>
+        <v>21.527000000000001</v>
       </c>
       <c r="O23" s="4"/>
       <c r="P23" s="5">
         <f>L23*N23/1000</f>
-        <v>1.9999320534320246</v>
+        <v>2.2790128509089942</v>
       </c>
       <c r="Q23" s="5"/>
       <c r="R23" s="5">
@@ -10089,27 +10055,27 @@
       </c>
       <c r="S23" s="5">
         <f>(C23*L23*1000/9.81)/D23</f>
-        <v>1.5341058904273392</v>
+        <v>1.7021780975370941</v>
       </c>
       <c r="T23" s="5">
         <f>(C23*L23*1000/9.81)/F23</f>
-        <v>0.93431617149945534</v>
+        <v>1.0366771506614003</v>
       </c>
       <c r="W23" s="5">
         <f>E23/(P23*C23)</f>
-        <v>1700.0577565449585</v>
+        <v>1491.873992129485</v>
       </c>
       <c r="Y23" s="5">
-        <f t="shared" ref="Y23:Y25" si="13">W23*0.33</f>
-        <v>561.01905965983633</v>
+        <f t="shared" si="13"/>
+        <v>492.31841740273006</v>
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B24" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -10126,12 +10092,12 @@
       <c r="G24" s="2">
         <v>23800</v>
       </c>
-      <c r="I24" s="3">
-        <v>0.76</v>
+      <c r="I24" s="6">
+        <v>0.6</v>
       </c>
       <c r="J24" s="3"/>
-      <c r="K24" s="2">
-        <v>459</v>
+      <c r="K24" s="7">
+        <v>450</v>
       </c>
       <c r="L24" s="4">
         <f>G24/224.809</f>
@@ -10139,17 +10105,17 @@
       </c>
       <c r="N24" s="4">
         <f>I24*28.325</f>
-        <v>21.527000000000001</v>
+        <v>16.994999999999997</v>
       </c>
       <c r="O24" s="4"/>
       <c r="P24" s="5">
         <f>L24*N24/1000</f>
-        <v>2.2790128509089942</v>
+        <v>1.7992206717702581</v>
       </c>
       <c r="Q24" s="5"/>
       <c r="R24" s="5">
         <f>K24/2.205</f>
-        <v>208.16326530612244</v>
+        <v>204.08163265306121</v>
       </c>
       <c r="S24" s="5">
         <f>(C24*L24*1000/9.81)/D24</f>
@@ -10161,93 +10127,29 @@
       </c>
       <c r="W24" s="5">
         <f>E24/(P24*C24)</f>
-        <v>1491.873992129485</v>
+        <v>1889.7070566973482</v>
       </c>
       <c r="Y24" s="5">
         <f t="shared" si="13"/>
-        <v>492.31841740273006</v>
-      </c>
-    </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>39</v>
-      </c>
-      <c r="B25" t="s">
-        <v>42</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="D25" s="8">
-        <v>6340</v>
-      </c>
-      <c r="E25" s="8">
-        <v>3400</v>
-      </c>
-      <c r="F25" s="8">
-        <v>10410</v>
-      </c>
-      <c r="G25" s="2">
-        <v>23800</v>
-      </c>
-      <c r="I25" s="6">
-        <v>0.6</v>
-      </c>
-      <c r="J25" s="3"/>
-      <c r="K25" s="7">
-        <v>450</v>
-      </c>
-      <c r="L25" s="4">
-        <f>G25/224.809</f>
-        <v>105.8676476475586</v>
-      </c>
-      <c r="N25" s="4">
-        <f>I25*28.325</f>
-        <v>16.994999999999997</v>
-      </c>
-      <c r="O25" s="4"/>
-      <c r="P25" s="5">
-        <f>L25*N25/1000</f>
-        <v>1.7992206717702581</v>
-      </c>
-      <c r="Q25" s="5"/>
-      <c r="R25" s="5">
-        <f>K25/2.205</f>
-        <v>204.08163265306121</v>
-      </c>
-      <c r="S25" s="5">
-        <f>(C25*L25*1000/9.81)/D25</f>
-        <v>1.7021780975370941</v>
-      </c>
-      <c r="T25" s="5">
-        <f>(C25*L25*1000/9.81)/F25</f>
-        <v>1.0366771506614003</v>
-      </c>
-      <c r="W25" s="5">
-        <f>E25/(P25*C25)</f>
-        <v>1889.7070566973482</v>
-      </c>
-      <c r="Y25" s="5">
-        <f t="shared" si="13"/>
         <v>623.60332871012497</v>
       </c>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>84</v>
+      </c>
+      <c r="G31" s="10" t="s">
         <v>85</v>
-      </c>
-      <c r="G31" s="10" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -10347,7 +10249,7 @@
         <v>75</v>
       </c>
       <c r="D2" s="1">
-        <f>IRL!$T$21</f>
+        <f>IRL!$T$20</f>
         <v>0.59648957438981809</v>
       </c>
       <c r="F2" t="s">
@@ -10361,7 +10263,7 @@
         <v>75</v>
       </c>
       <c r="I2">
-        <f>IRL!$T$23</f>
+        <f>IRL!$T$22</f>
         <v>0.93431617149945534</v>
       </c>
       <c r="K2" t="s">
@@ -10375,7 +10277,7 @@
         <v>75</v>
       </c>
       <c r="N2">
-        <f>IRL!$T$24</f>
+        <f>IRL!$T$23</f>
         <v>1.0366771506614003</v>
       </c>
       <c r="P2" t="s">
@@ -10389,7 +10291,7 @@
         <v>75</v>
       </c>
       <c r="S2">
-        <f>IRL!$T$25</f>
+        <f>IRL!$T$24</f>
         <v>1.0366771506614003</v>
       </c>
     </row>
@@ -10445,60 +10347,60 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4">
-        <f>IRL!$L$21*1000</f>
+        <f>IRL!$L$20*1000</f>
         <v>40323.118736349519</v>
       </c>
       <c r="B4">
-        <f>IRL!$R$21</f>
+        <f>IRL!$R$20</f>
         <v>151.0204081632653</v>
       </c>
       <c r="C4">
-        <f>IRL!$P$21</f>
+        <f>IRL!$P$20</f>
         <v>0.42259636513662707</v>
       </c>
       <c r="D4">
         <v>1000</v>
       </c>
       <c r="F4">
+        <f>IRL!$L$22*1000</f>
+        <v>95414.329497484534</v>
+      </c>
+      <c r="G4">
+        <f>IRL!$R$22</f>
+        <v>208.16326530612244</v>
+      </c>
+      <c r="H4">
+        <f>IRL!$P$22</f>
+        <v>1.9999320534320246</v>
+      </c>
+      <c r="I4">
+        <v>1500</v>
+      </c>
+      <c r="K4">
         <f>IRL!$L$23*1000</f>
-        <v>95414.329497484534</v>
-      </c>
-      <c r="G4">
+        <v>105867.6476475586</v>
+      </c>
+      <c r="L4">
         <f>IRL!$R$23</f>
         <v>208.16326530612244</v>
       </c>
-      <c r="H4">
+      <c r="M4">
         <f>IRL!$P$23</f>
-        <v>1.9999320534320246</v>
-      </c>
-      <c r="I4">
+        <v>2.2790128509089942</v>
+      </c>
+      <c r="N4">
         <v>1500</v>
       </c>
-      <c r="K4">
+      <c r="P4">
         <f>IRL!$L$24*1000</f>
         <v>105867.6476475586</v>
       </c>
-      <c r="L4">
+      <c r="Q4">
         <f>IRL!$R$24</f>
-        <v>208.16326530612244</v>
-      </c>
-      <c r="M4">
+        <v>204.08163265306121</v>
+      </c>
+      <c r="R4">
         <f>IRL!$P$24</f>
-        <v>2.2790128509089942</v>
-      </c>
-      <c r="N4">
-        <v>1500</v>
-      </c>
-      <c r="P4">
-        <f>IRL!$L$25*1000</f>
-        <v>105867.6476475586</v>
-      </c>
-      <c r="Q4">
-        <f>IRL!$R$25</f>
-        <v>204.08163265306121</v>
-      </c>
-      <c r="R4">
-        <f>IRL!$P$25</f>
         <v>1.7992206717702581</v>
       </c>
       <c r="S4">
@@ -11999,7 +11901,7 @@
         <v>150</v>
       </c>
       <c r="D32">
-        <f>IRL!$V$13</f>
+        <f>IRL!$V$12</f>
         <v>1.0706378260240621</v>
       </c>
       <c r="F32" t="s">
@@ -12013,7 +11915,7 @@
         <v>150</v>
       </c>
       <c r="I32">
-        <f>IRL!$V$14</f>
+        <f>IRL!$V$13</f>
         <v>0.9396010660128562</v>
       </c>
       <c r="K32" t="s">
@@ -12027,7 +11929,7 @@
         <v>150</v>
       </c>
       <c r="N32">
-        <f>IRL!$V$15</f>
+        <f>IRL!$V$14</f>
         <v>1.1040213952312201</v>
       </c>
       <c r="P32" t="s">
@@ -12041,7 +11943,7 @@
         <v>150</v>
       </c>
       <c r="S32">
-        <f>IRL!$V$16</f>
+        <f>IRL!$V$15</f>
         <v>1.1473936643295894</v>
       </c>
     </row>
@@ -12097,60 +11999,60 @@
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A34">
+        <f>IRL!$L$12*1000</f>
+        <v>65255.394579398511</v>
+      </c>
+      <c r="B34">
+        <f>IRL!$R$12</f>
+        <v>103.40136054421768</v>
+      </c>
+      <c r="C34">
+        <f>IRL!$P$12</f>
+        <v>1.358543902824175</v>
+      </c>
+      <c r="D34">
+        <v>3000</v>
+      </c>
+      <c r="F34">
         <f>IRL!$L$13*1000</f>
         <v>65255.394579398511</v>
       </c>
-      <c r="B34">
+      <c r="G34">
         <f>IRL!$R$13</f>
         <v>103.40136054421768</v>
       </c>
-      <c r="C34">
+      <c r="H34">
         <f>IRL!$P$13</f>
         <v>1.358543902824175</v>
       </c>
-      <c r="D34">
-        <v>3000</v>
-      </c>
-      <c r="F34">
-        <f>IRL!$L$14*1000</f>
-        <v>65255.394579398511</v>
-      </c>
-      <c r="G34">
-        <f>IRL!$R$14</f>
-        <v>103.40136054421768</v>
-      </c>
-      <c r="H34">
-        <f>IRL!$P$14</f>
-        <v>1.358543902824175</v>
-      </c>
       <c r="I34">
         <v>3000</v>
       </c>
       <c r="K34">
-        <f>IRL!$L$15*1000</f>
+        <f>IRL!$L$14*1000</f>
         <v>75619.748319684717</v>
       </c>
       <c r="L34">
-        <f>IRL!$R$15</f>
+        <f>IRL!$R$14</f>
         <v>122.44897959183673</v>
       </c>
       <c r="M34">
-        <f>IRL!$P$15</f>
+        <f>IRL!$P$14</f>
         <v>1.5957373815105271</v>
       </c>
       <c r="N34">
         <v>3000</v>
       </c>
       <c r="P34">
-        <f>IRL!$L$16*1000</f>
+        <f>IRL!$L$15*1000</f>
         <v>79178.324711199282</v>
       </c>
       <c r="Q34">
-        <f>IRL!$R$16</f>
+        <f>IRL!$R$15</f>
         <v>115.19274376417233</v>
       </c>
       <c r="R34">
-        <f>IRL!$P$16</f>
+        <f>IRL!$P$15</f>
         <v>1.6282191104448664</v>
       </c>
       <c r="S34">
@@ -13651,7 +13553,7 @@
         <v>150</v>
       </c>
       <c r="D62">
-        <f>IRL!$V$8</f>
+        <f>IRL!$V$7</f>
         <v>1.0562600703127314</v>
       </c>
       <c r="F62" t="s">
@@ -13665,7 +13567,7 @@
         <v>150</v>
       </c>
       <c r="I62">
-        <f>IRL!$V$9</f>
+        <f>IRL!$V$8</f>
         <v>1.093983644252472</v>
       </c>
       <c r="K62" t="s">
@@ -13679,7 +13581,7 @@
         <v>150</v>
       </c>
       <c r="N62">
-        <f>IRL!$V$10</f>
+        <f>IRL!$V$9</f>
         <v>0.89895276698401383</v>
       </c>
       <c r="P62" t="s">
@@ -13693,7 +13595,7 @@
         <v>150</v>
       </c>
       <c r="S62">
-        <f>IRL!$V$11</f>
+        <f>IRL!$V$10</f>
         <v>1.0977560016464458</v>
       </c>
     </row>
@@ -13749,60 +13651,60 @@
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A64">
-        <f>IRL!$L$8*1000</f>
+        <f>IRL!$L$7*1000</f>
         <v>73840.460123927434</v>
       </c>
       <c r="B64">
-        <f>IRL!$R$8</f>
+        <f>IRL!$R$7</f>
         <v>119.72789115646258</v>
       </c>
       <c r="C64">
-        <f>IRL!$P$8</f>
+        <f>IRL!$P$7</f>
         <v>1.5581906195926323</v>
       </c>
       <c r="D64">
         <v>3000</v>
       </c>
       <c r="F64">
-        <f>IRL!$L$9*1000</f>
+        <f>IRL!$L$8*1000</f>
         <v>75619.748319684717</v>
       </c>
       <c r="G64">
-        <f>IRL!$R$9</f>
+        <f>IRL!$R$8</f>
         <v>122.44897959183673</v>
       </c>
       <c r="H64">
-        <f>IRL!$P$9</f>
+        <f>IRL!$P$8</f>
         <v>1.5957373815105271</v>
       </c>
       <c r="I64">
         <v>3000</v>
       </c>
       <c r="K64">
-        <f>IRL!$L$10*1000</f>
+        <f>IRL!$L$9*1000</f>
         <v>65255.394579398511</v>
       </c>
       <c r="L64">
-        <f>IRL!$R$10</f>
+        <f>IRL!$R$9</f>
         <v>103.40136054421768</v>
       </c>
       <c r="M64">
-        <f>IRL!$P$10</f>
+        <f>IRL!$P$9</f>
         <v>1.358543902824175</v>
       </c>
       <c r="N64">
         <v>3000</v>
       </c>
       <c r="P64">
-        <f>IRL!$L$11*1000</f>
+        <f>IRL!$L$10*1000</f>
         <v>79178.324711199282</v>
       </c>
       <c r="Q64">
-        <f>IRL!$R$11</f>
+        <f>IRL!$R$10</f>
         <v>115.19274376417233</v>
       </c>
       <c r="R64">
-        <f>IRL!$P$11</f>
+        <f>IRL!$P$10</f>
         <v>1.6282191104448664</v>
       </c>
       <c r="S64">
@@ -15291,7 +15193,7 @@
         <v>150</v>
       </c>
       <c r="D92">
-        <f>IRL!$V$18</f>
+        <f>IRL!$V$17</f>
         <v>0.68501505641647376</v>
       </c>
       <c r="F92" t="s">
@@ -15305,7 +15207,7 @@
         <v>150</v>
       </c>
       <c r="I92">
-        <f>IRL!$V$19</f>
+        <f>IRL!$V$18</f>
         <v>0.85479390771969554</v>
       </c>
       <c r="K92" t="s">
@@ -15363,30 +15265,30 @@
     </row>
     <row r="94" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A94">
-        <f>IRL!$L$18*1000</f>
+        <f>IRL!$L$17*1000</f>
         <v>54935.523044006244</v>
       </c>
       <c r="B94">
-        <f>IRL!$R$18</f>
+        <f>IRL!$R$17</f>
         <v>117.91383219954648</v>
       </c>
       <c r="C94">
-        <f>IRL!$P$18</f>
+        <f>IRL!$P$17</f>
         <v>1.0378844763777251</v>
       </c>
       <c r="D94">
         <v>3000</v>
       </c>
       <c r="F94">
-        <f>IRL!$L$19*1000</f>
+        <f>IRL!$L$18*1000</f>
         <v>74730.104221806076</v>
       </c>
       <c r="G94">
-        <f>IRL!$R$19</f>
+        <f>IRL!$R$18</f>
         <v>113.37868480725623</v>
       </c>
       <c r="H94">
-        <f>IRL!$P$19</f>
+        <f>IRL!$P$18</f>
         <v>1.5769640005515797</v>
       </c>
       <c r="I94">

</xml_diff>

<commit_message>
Try doubling A-10 thrust
</commit_message>
<xml_diff>
--- a/REB Engine Profile.xlsx
+++ b/REB Engine Profile.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgkid\Documents\GitHub\REBalanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7116093D-ECB3-4FF6-9233-14B2A411DC16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31A8A399-0249-414D-A1E3-0F663CDF8B10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{48F6B32E-432E-46EB-935F-18F86645025F}"/>
   </bookViews>
@@ -34,6 +34,42 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={5F58F688-8559-4CAA-903D-5B37486DED4F}</author>
+  </authors>
+  <commentList>
+    <comment ref="G20" authorId="0" shapeId="0" xr:uid="{5F58F688-8559-4CAA-903D-5B37486DED4F}">
+      <text>
+        <t>[스레드 댓글]
+사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
+댓글:
+    9065 lbs is correct value, but for viable gameplay it is set to current value.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={FDD360BB-6FD3-4C03-907D-93C92009B2A2}</author>
+  </authors>
+  <commentList>
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{FDD360BB-6FD3-4C03-907D-93C92009B2A2}">
+      <text>
+        <t>[스레드 댓글]
+사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
+댓글:
+    IRL it's more like 1000</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -379,7 +415,7 @@
     <numFmt numFmtId="179" formatCode="#,##0.0000_ "/>
     <numFmt numFmtId="180" formatCode="#,##0.00_ "/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -416,6 +452,12 @@
       <sz val="11"/>
       <color rgb="FF202122"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -536,7 +578,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -564,16 +606,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
@@ -594,19 +630,10 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
@@ -633,15 +660,6 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -662,6 +680,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6401,52 +6428,52 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>5.8515627247641158</c:v>
+                  <c:v>11.703125449528232</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.432984674794004</c:v>
+                  <c:v>11.012806773231089</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.0484046673105487</c:v>
+                  <c:v>10.393774315051131</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.687952302882139</c:v>
+                  <c:v>9.8295774092690014</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.3417571820771643</c:v>
+                  <c:v>9.3037653901653528</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.9999489054640169</c:v>
+                  <c:v>8.7998875920208377</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.652657073611087</c:v>
+                  <c:v>8.3014933491161056</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.290011287086763</c:v>
+                  <c:v>7.7921319957318076</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.9021411464594378</c:v>
+                  <c:v>7.255352866148594</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.4791762522974996</c:v>
+                  <c:v>6.674705294647115</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.0112462051693405</c:v>
+                  <c:v>6.033738615508021</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.4884806056433504</c:v>
+                  <c:v>5.3160021630119649</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.90100905428791878</c:v>
+                  <c:v>4.5050452714395952</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.23896115167143778</c:v>
+                  <c:v>3.5844172750715635</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>2.5376675081885196</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>1.3483453050711149</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>0</c:v>
@@ -8294,7 +8321,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{56A8DD58-7ECC-479E-88D8-A0EAF35ACF06}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="118" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="124" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8305,7 +8332,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9298983" cy="6078242"/>
+    <xdr:ext cx="9302238" cy="6083710"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="차트 1">
@@ -8334,10 +8361,16 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Mingi Park" id="{2B9CBCF4-6017-4503-A8D7-215C7F85D903}" userId="cd0a2b2004dc7eb2" providerId="Windows Live"/>
+</personList>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 테마">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -8375,7 +8408,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -8481,7 +8514,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -8623,18 +8656,34 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="G20" dT="2024-03-24T11:53:42.82" personId="{2B9CBCF4-6017-4503-A8D7-215C7F85D903}" id="{5F58F688-8559-4CAA-903D-5B37486DED4F}">
+    <text>9065 lbs is correct value, but for viable gameplay it is set to current value.</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="D4" dT="2024-03-24T11:58:52.86" personId="{2B9CBCF4-6017-4503-A8D7-215C7F85D903}" id="{FDD360BB-6FD3-4C03-907D-93C92009B2A2}">
+    <text>IRL it's more like 1000</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FFD454E-F3C6-4FAB-86B6-C320D531FCD7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FFD454E-F3C6-4FAB-86B6-C320D531FCD7}">
   <dimension ref="A1:Z32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -8666,116 +8715,116 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="32" t="s">
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
-      <c r="O1" s="33"/>
-      <c r="P1" s="33"/>
-      <c r="Q1" s="33"/>
-      <c r="R1" s="34"/>
-      <c r="S1" s="33" t="s">
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="35"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="T1" s="33"/>
-      <c r="U1" s="33"/>
-      <c r="V1" s="33"/>
-      <c r="W1" s="33"/>
-      <c r="X1" s="33"/>
-      <c r="Y1" s="33"/>
-      <c r="Z1" s="34"/>
+      <c r="T1" s="35"/>
+      <c r="U1" s="35"/>
+      <c r="V1" s="35"/>
+      <c r="W1" s="35"/>
+      <c r="X1" s="35"/>
+      <c r="Y1" s="35"/>
+      <c r="Z1" s="36"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="40" t="s">
+      <c r="E2" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="F2" s="41" t="s">
+      <c r="F2" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="G2" s="39" t="s">
+      <c r="G2" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="H2" s="40" t="s">
+      <c r="H2" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="I2" s="40" t="s">
+      <c r="I2" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="J2" s="40" t="s">
+      <c r="J2" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="K2" s="41" t="s">
+      <c r="K2" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="L2" s="40" t="s">
+      <c r="L2" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="M2" s="40" t="s">
+      <c r="M2" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="N2" s="40" t="s">
+      <c r="N2" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="O2" s="40" t="s">
+      <c r="O2" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="P2" s="40" t="s">
+      <c r="P2" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="Q2" s="40" t="s">
+      <c r="Q2" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="R2" s="41" t="s">
+      <c r="R2" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="S2" s="39" t="s">
+      <c r="S2" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="T2" s="40" t="s">
+      <c r="T2" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="U2" s="40" t="s">
+      <c r="U2" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="V2" s="40" t="s">
+      <c r="V2" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="W2" s="40" t="s">
+      <c r="W2" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="X2" s="40" t="s">
+      <c r="X2" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="Y2" s="40" t="s">
+      <c r="Y2" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="Z2" s="41" t="s">
+      <c r="Z2" s="33" t="s">
         <v>71</v>
       </c>
     </row>
@@ -8783,93 +8832,93 @@
       <c r="A3" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3">
         <v>2</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="2">
         <v>10660</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="2">
         <v>4930</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="9">
         <v>16769</v>
       </c>
-      <c r="G3" s="18">
+      <c r="G3" s="16">
         <v>10600</v>
       </c>
-      <c r="H3" s="10">
+      <c r="H3" s="2">
         <v>16000</v>
       </c>
-      <c r="I3" s="19">
+      <c r="I3" s="3">
         <v>0.85299999999999998</v>
       </c>
-      <c r="J3" s="19">
+      <c r="J3" s="3">
         <v>1.85</v>
       </c>
-      <c r="K3" s="11">
+      <c r="K3" s="9">
         <v>142</v>
       </c>
-      <c r="L3" s="20">
+      <c r="L3" s="4">
         <f t="shared" ref="L3:M5" si="0">G3/224.809</f>
         <v>47.151137187568111</v>
       </c>
-      <c r="M3" s="20">
+      <c r="M3" s="4">
         <f t="shared" si="0"/>
         <v>71.171527830291495</v>
       </c>
-      <c r="N3" s="20">
+      <c r="N3" s="4">
         <f t="shared" ref="N3:O5" si="1">I3*28.325</f>
         <v>24.161224999999998</v>
       </c>
-      <c r="O3" s="20">
+      <c r="O3" s="4">
         <f t="shared" si="1"/>
         <v>52.401250000000005</v>
       </c>
-      <c r="P3" s="21">
+      <c r="P3" s="5">
         <f t="shared" ref="P3:Q5" si="2">L3*N3/1000</f>
         <v>1.1392292345947004</v>
       </c>
-      <c r="Q3" s="21">
+      <c r="Q3" s="5">
         <f t="shared" si="2"/>
         <v>3.7294770227170626</v>
       </c>
-      <c r="R3" s="22">
+      <c r="R3" s="17">
         <f>K3/2.205</f>
         <v>64.399092970521536</v>
       </c>
-      <c r="S3" s="35">
+      <c r="S3" s="27">
         <f>(C3*L3*1000/9.81)/D3</f>
         <v>0.90177035700003838</v>
       </c>
-      <c r="T3" s="21">
+      <c r="T3" s="5">
         <f>(C3*L3*1000/9.81)/F3</f>
         <v>0.57325254968217598</v>
       </c>
-      <c r="U3" s="21">
+      <c r="U3" s="5">
         <f>(C3*M3*1000/9.81)/D3</f>
         <v>1.361162803018926</v>
       </c>
-      <c r="V3" s="21">
+      <c r="V3" s="5">
         <f>(C3*M3*1000/9.81)/F3</f>
         <v>0.86528686744479399</v>
       </c>
-      <c r="W3" s="21">
+      <c r="W3" s="5">
         <f>E3/(P3*C3)</f>
         <v>2163.743630470442</v>
       </c>
-      <c r="X3" s="21">
+      <c r="X3" s="5">
         <f>E3/(Q3*C3)</f>
         <v>660.95057966174465</v>
       </c>
-      <c r="Y3" s="21">
+      <c r="Y3" s="5">
         <f>W3*0.33</f>
         <v>714.03539805524588</v>
       </c>
-      <c r="Z3" s="22">
+      <c r="Z3" s="17">
         <f>Q3/P3</f>
         <v>3.2736844433630479</v>
       </c>
@@ -8878,93 +8927,93 @@
       <c r="A4" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4">
         <v>2</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="2">
         <v>10433</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="2">
         <v>4930</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="9">
         <v>16769</v>
       </c>
-      <c r="G4" s="18">
+      <c r="G4" s="16">
         <v>11950</v>
       </c>
-      <c r="H4" s="10">
+      <c r="H4" s="2">
         <v>17700</v>
       </c>
-      <c r="I4" s="23">
+      <c r="I4" s="18">
         <v>0.85299999999999998</v>
       </c>
-      <c r="J4" s="19">
+      <c r="J4" s="3">
         <v>1.74</v>
       </c>
-      <c r="K4" s="11">
+      <c r="K4" s="9">
         <v>146</v>
       </c>
-      <c r="L4" s="20">
+      <c r="L4" s="4">
         <f t="shared" si="0"/>
         <v>53.156234848248957</v>
       </c>
-      <c r="M4" s="20">
+      <c r="M4" s="4">
         <f t="shared" si="0"/>
         <v>78.733502662259966</v>
       </c>
-      <c r="N4" s="20">
+      <c r="N4" s="4">
         <f t="shared" si="1"/>
         <v>24.161224999999998</v>
       </c>
-      <c r="O4" s="20">
+      <c r="O4" s="4">
         <f t="shared" si="1"/>
         <v>49.285499999999999</v>
       </c>
-      <c r="P4" s="21">
+      <c r="P4" s="5">
         <f t="shared" si="2"/>
         <v>1.2843197503213837</v>
       </c>
-      <c r="Q4" s="21">
+      <c r="Q4" s="5">
         <f t="shared" si="2"/>
         <v>3.8804200454608133</v>
       </c>
-      <c r="R4" s="22">
+      <c r="R4" s="17">
         <f>K4/2.205</f>
         <v>66.213151927437636</v>
       </c>
-      <c r="S4" s="35">
+      <c r="S4" s="27">
         <f>(C4*L4*1000/9.81)/D4</f>
         <v>1.038737934847191</v>
       </c>
-      <c r="T4" s="21">
+      <c r="T4" s="5">
         <f>(C4*L4*1000/9.81)/F4</f>
         <v>0.64626112912283051</v>
       </c>
-      <c r="U4" s="21">
+      <c r="U4" s="5">
         <f>(C4*M4*1000/9.81)/D4</f>
         <v>1.5385490750456305</v>
       </c>
-      <c r="V4" s="21">
+      <c r="V4" s="5">
         <f>(C4*M4*1000/9.81)/F4</f>
         <v>0.9572235971108034</v>
       </c>
-      <c r="W4" s="21">
+      <c r="W4" s="5">
         <f>E4/(P4*C4)</f>
         <v>1919.3039734716897</v>
       </c>
-      <c r="X4" s="21">
+      <c r="X4" s="5">
         <f>E4/(Q4*C4)</f>
         <v>635.24050775984301</v>
       </c>
-      <c r="Y4" s="21">
+      <c r="Y4" s="5">
         <f t="shared" ref="Y4:Y5" si="3">W4*0.33</f>
         <v>633.3703112456576</v>
       </c>
-      <c r="Z4" s="22">
+      <c r="Z4" s="17">
         <f>Q4/P4</f>
         <v>3.0213815870150644</v>
       </c>
@@ -8973,216 +9022,202 @@
       <c r="A5" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" t="s">
         <v>76</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5">
         <v>2</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="2">
         <v>14552</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="2">
         <v>6667</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="9">
         <v>23000</v>
       </c>
-      <c r="G5" s="18">
+      <c r="G5" s="16">
         <v>12500</v>
       </c>
-      <c r="H5" s="10">
+      <c r="H5" s="2">
         <v>22000</v>
       </c>
-      <c r="I5" s="23">
+      <c r="I5" s="18">
         <v>0.72399999999999998</v>
       </c>
-      <c r="J5" s="23">
+      <c r="J5" s="18">
         <v>1.8</v>
       </c>
-      <c r="K5" s="11">
+      <c r="K5" s="9">
         <v>169</v>
       </c>
-      <c r="L5" s="20">
+      <c r="L5" s="4">
         <f t="shared" si="0"/>
         <v>55.602756117415225</v>
       </c>
-      <c r="M5" s="20">
+      <c r="M5" s="4">
         <f t="shared" si="0"/>
         <v>97.860850766650799</v>
       </c>
-      <c r="N5" s="20">
+      <c r="N5" s="4">
         <f t="shared" si="1"/>
         <v>20.507299999999997</v>
       </c>
-      <c r="O5" s="20">
+      <c r="O5" s="4">
         <f t="shared" si="1"/>
         <v>50.984999999999999</v>
       </c>
-      <c r="P5" s="21">
+      <c r="P5" s="5">
         <f t="shared" si="2"/>
         <v>1.1402624005266691</v>
       </c>
-      <c r="Q5" s="21">
+      <c r="Q5" s="5">
         <f t="shared" si="2"/>
         <v>4.9894354763376905</v>
       </c>
-      <c r="R5" s="22">
+      <c r="R5" s="17">
         <f>K5/2.205</f>
         <v>76.643990929705211</v>
       </c>
-      <c r="S5" s="35">
+      <c r="S5" s="27">
         <f>(C5*L5*1000/9.81)/D5</f>
         <v>0.77899491265063181</v>
       </c>
-      <c r="T5" s="21">
+      <c r="T5" s="5">
         <f>(C5*L5*1000/9.81)/F5</f>
         <v>0.49286669429965191</v>
       </c>
-      <c r="U5" s="21">
+      <c r="U5" s="5">
         <f>(C5*M5*1000/9.81)/D5</f>
         <v>1.3710310462651119</v>
       </c>
-      <c r="V5" s="21">
+      <c r="V5" s="5">
         <f>(C5*M5*1000/9.81)/F5</f>
         <v>0.86744538196738719</v>
       </c>
-      <c r="W5" s="21">
+      <c r="W5" s="5">
         <f>E5/(P5*C5)</f>
         <v>2923.4498993041507</v>
       </c>
-      <c r="X5" s="21">
+      <c r="X5" s="5">
         <f>E5/(Q5*C5)</f>
         <v>668.1116562803677</v>
       </c>
-      <c r="Y5" s="21">
+      <c r="Y5" s="5">
         <f t="shared" si="3"/>
         <v>964.73846677036977</v>
       </c>
-      <c r="Z5" s="22">
+      <c r="Z5" s="17">
         <f>Q5/P5</f>
         <v>4.375690607734807</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" s="8"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="20"/>
-      <c r="M6" s="20"/>
-      <c r="N6" s="20"/>
-      <c r="O6" s="20"/>
-      <c r="P6" s="21"/>
-      <c r="Q6" s="21"/>
-      <c r="R6" s="22"/>
-      <c r="S6" s="35"/>
-      <c r="T6" s="21"/>
-      <c r="U6" s="21"/>
-      <c r="V6" s="21"/>
-      <c r="W6" s="21"/>
-      <c r="X6" s="21"/>
-      <c r="Y6" s="21"/>
-      <c r="Z6" s="22"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="16"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="17"/>
+      <c r="S6" s="27"/>
+      <c r="Z6" s="17"/>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7">
         <v>1</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="2">
         <v>8573</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="2">
         <v>3200</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="9">
         <v>12020</v>
       </c>
-      <c r="G7" s="18">
+      <c r="G7" s="16">
         <v>16600</v>
       </c>
-      <c r="H7" s="10">
+      <c r="H7" s="2">
         <v>28000</v>
       </c>
-      <c r="I7" s="19">
+      <c r="I7" s="3">
         <v>0.745</v>
       </c>
-      <c r="J7" s="19">
+      <c r="J7" s="3">
         <v>1.9710000000000001</v>
       </c>
-      <c r="K7" s="11">
+      <c r="K7" s="9">
         <v>264</v>
       </c>
-      <c r="L7" s="20">
+      <c r="L7" s="4">
         <f t="shared" ref="L7:M10" si="4">G7/224.809</f>
         <v>73.840460123927429</v>
       </c>
-      <c r="M7" s="20">
+      <c r="M7" s="4">
         <f t="shared" si="4"/>
         <v>124.55017370301012</v>
       </c>
-      <c r="N7" s="20">
+      <c r="N7" s="4">
         <f t="shared" ref="N7:O10" si="5">I7*28.325</f>
         <v>21.102125000000001</v>
       </c>
-      <c r="O7" s="20">
+      <c r="O7" s="4">
         <f t="shared" si="5"/>
         <v>55.828575000000001</v>
       </c>
-      <c r="P7" s="21">
+      <c r="P7" s="5">
         <f t="shared" ref="P7:Q10" si="6">L7*N7/1000</f>
         <v>1.5581906195926323</v>
       </c>
-      <c r="Q7" s="21">
+      <c r="Q7" s="5">
         <f t="shared" si="6"/>
         <v>6.9534587138415285</v>
       </c>
-      <c r="R7" s="22">
+      <c r="R7" s="17">
         <f>K7/2.205</f>
         <v>119.72789115646258</v>
       </c>
-      <c r="S7" s="35">
+      <c r="S7" s="27">
         <f>(C7*L7*1000/9.81)/D7</f>
         <v>0.87799605218060006</v>
       </c>
-      <c r="T7" s="21">
+      <c r="T7" s="5">
         <f>(C7*L7*1000/9.81)/F7</f>
         <v>0.62621132739969088</v>
       </c>
-      <c r="U7" s="21">
+      <c r="U7" s="5">
         <f>(C7*M7*1000/9.81)/D7</f>
         <v>1.4809571964492048</v>
       </c>
-      <c r="V7" s="21">
+      <c r="V7" s="5">
         <f>(C7*M7*1000/9.81)/F7</f>
         <v>1.0562600703127314</v>
       </c>
-      <c r="W7" s="21">
+      <c r="W7" s="5">
         <f>E7/(P7*C7)</f>
         <v>2053.6640124534933</v>
       </c>
-      <c r="X7" s="21">
+      <c r="X7" s="5">
         <f>E7/(Q7*C7)</f>
         <v>460.20263176799943</v>
       </c>
-      <c r="Y7" s="21">
+      <c r="Y7" s="5">
         <f t="shared" ref="Y7" si="7">W7*0.33</f>
         <v>677.70912410965286</v>
       </c>
-      <c r="Z7" s="22">
+      <c r="Z7" s="17">
         <f>Q7/P7</f>
         <v>4.462521225842969</v>
       </c>
@@ -9191,93 +9226,93 @@
       <c r="A8" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8">
         <v>1</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="2">
         <v>8573</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="2">
         <v>3200</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="9">
         <v>12020</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="16">
         <v>17000</v>
       </c>
-      <c r="H8" s="10">
+      <c r="H8" s="2">
         <v>29000</v>
       </c>
-      <c r="I8" s="23">
+      <c r="I8" s="18">
         <v>0.745</v>
       </c>
-      <c r="J8" s="19">
+      <c r="J8" s="3">
         <v>1.9</v>
       </c>
-      <c r="K8" s="11">
+      <c r="K8" s="9">
         <v>270</v>
       </c>
-      <c r="L8" s="20">
+      <c r="L8" s="4">
         <f t="shared" si="4"/>
         <v>75.619748319684717</v>
       </c>
-      <c r="M8" s="20">
+      <c r="M8" s="4">
         <f t="shared" si="4"/>
         <v>128.99839419240334</v>
       </c>
-      <c r="N8" s="20">
+      <c r="N8" s="4">
         <f t="shared" si="5"/>
         <v>21.102125000000001</v>
       </c>
-      <c r="O8" s="20">
+      <c r="O8" s="4">
         <f t="shared" si="5"/>
         <v>53.817499999999995</v>
       </c>
-      <c r="P8" s="21">
+      <c r="P8" s="5">
         <f t="shared" si="6"/>
         <v>1.5957373815105271</v>
       </c>
-      <c r="Q8" s="21">
+      <c r="Q8" s="5">
         <f t="shared" si="6"/>
         <v>6.942371079449666</v>
       </c>
-      <c r="R8" s="22">
+      <c r="R8" s="17">
         <f>K8/2.205</f>
         <v>122.44897959183673</v>
       </c>
-      <c r="S8" s="35">
+      <c r="S8" s="27">
         <f>(C8*L8*1000/9.81)/D8</f>
         <v>0.89915258355844574</v>
       </c>
-      <c r="T8" s="21">
+      <c r="T8" s="5">
         <f>(C8*L8*1000/9.81)/F8</f>
         <v>0.64130075697558697</v>
       </c>
-      <c r="U8" s="21">
+      <c r="U8" s="5">
         <f>(C8*M8*1000/9.81)/D8</f>
         <v>1.5338485248938192</v>
       </c>
-      <c r="V8" s="21">
+      <c r="V8" s="5">
         <f>(C8*M8*1000/9.81)/F8</f>
         <v>1.093983644252472</v>
       </c>
-      <c r="W8" s="21">
+      <c r="W8" s="5">
         <f>E8/(P8*C8)</f>
         <v>2005.3425062781168</v>
       </c>
-      <c r="X8" s="21">
+      <c r="X8" s="5">
         <f>E8/(Q8*C8)</f>
         <v>460.93761963724785</v>
       </c>
-      <c r="Y8" s="21">
+      <c r="Y8" s="5">
         <f>W8*0.33</f>
         <v>661.76302707177854</v>
       </c>
-      <c r="Z8" s="22">
+      <c r="Z8" s="17">
         <f>Q8/P8</f>
         <v>4.3505724437425961</v>
       </c>
@@ -9286,93 +9321,93 @@
       <c r="A9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" t="s">
         <v>78</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9">
         <v>1</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="2">
         <v>8573</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="2">
         <v>3200</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="9">
         <v>12020</v>
       </c>
-      <c r="G9" s="18">
+      <c r="G9" s="16">
         <v>14670</v>
       </c>
-      <c r="H9" s="10">
+      <c r="H9" s="2">
         <v>23830</v>
       </c>
-      <c r="I9" s="23">
+      <c r="I9" s="18">
         <v>0.73499999999999999</v>
       </c>
-      <c r="J9" s="19">
+      <c r="J9" s="3">
         <v>2.1</v>
       </c>
-      <c r="K9" s="11">
+      <c r="K9" s="9">
         <v>228</v>
       </c>
-      <c r="L9" s="20">
+      <c r="L9" s="4">
         <f t="shared" si="4"/>
         <v>65.255394579398512</v>
       </c>
-      <c r="M9" s="20">
+      <c r="M9" s="4">
         <f t="shared" si="4"/>
         <v>106.00109426224039</v>
       </c>
-      <c r="N9" s="20">
+      <c r="N9" s="4">
         <f t="shared" si="5"/>
         <v>20.818874999999998</v>
       </c>
-      <c r="O9" s="20">
+      <c r="O9" s="4">
         <f t="shared" si="5"/>
         <v>59.482500000000002</v>
       </c>
-      <c r="P9" s="21">
+      <c r="P9" s="5">
         <f t="shared" si="6"/>
         <v>1.358543902824175</v>
       </c>
-      <c r="Q9" s="21">
+      <c r="Q9" s="5">
         <f t="shared" si="6"/>
         <v>6.3052100894537144</v>
       </c>
-      <c r="R9" s="22">
+      <c r="R9" s="17">
         <f>K9/2.205</f>
         <v>103.40136054421768</v>
       </c>
-      <c r="S9" s="35">
+      <c r="S9" s="27">
         <f>(C9*L9*1000/9.81)/D9</f>
         <v>0.77591578828249408</v>
       </c>
-      <c r="T9" s="21">
+      <c r="T9" s="5">
         <f>(C9*L9*1000/9.81)/F9</f>
         <v>0.55340482969599181</v>
       </c>
-      <c r="U9" s="21">
+      <c r="U9" s="5">
         <f>(C9*M9*1000/9.81)/D9</f>
         <v>1.2604003568351623</v>
       </c>
-      <c r="V9" s="21">
+      <c r="V9" s="5">
         <f>(C9*M9*1000/9.81)/F9</f>
         <v>0.89895276698401383</v>
       </c>
-      <c r="W9" s="21">
+      <c r="W9" s="5">
         <f>E9/(P9*C9)</f>
         <v>2355.4630758327057</v>
       </c>
-      <c r="X9" s="21">
+      <c r="X9" s="5">
         <f>E9/(Q9*C9)</f>
         <v>507.51679239878416</v>
       </c>
-      <c r="Y9" s="21">
+      <c r="Y9" s="5">
         <f>W9*0.33</f>
         <v>777.30281502479295</v>
       </c>
-      <c r="Z9" s="22">
+      <c r="Z9" s="17">
         <f>Q9/P9</f>
         <v>4.641152984711268</v>
       </c>
@@ -9381,216 +9416,202 @@
       <c r="A10" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10">
         <v>1</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="2">
         <v>8573</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="2">
         <v>3200</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="9">
         <v>12020</v>
       </c>
-      <c r="G10" s="18">
+      <c r="G10" s="16">
         <v>17800</v>
       </c>
-      <c r="H10" s="10">
+      <c r="H10" s="2">
         <v>29100</v>
       </c>
-      <c r="I10" s="19">
+      <c r="I10" s="3">
         <v>0.72599999999999998</v>
       </c>
-      <c r="J10" s="19">
+      <c r="J10" s="3">
         <v>2.06</v>
       </c>
-      <c r="K10" s="11">
+      <c r="K10" s="9">
         <v>254</v>
       </c>
-      <c r="L10" s="20">
+      <c r="L10" s="4">
         <f t="shared" si="4"/>
         <v>79.178324711199281</v>
       </c>
-      <c r="M10" s="20">
+      <c r="M10" s="4">
         <f t="shared" si="4"/>
         <v>129.44321624134264</v>
       </c>
-      <c r="N10" s="20">
+      <c r="N10" s="4">
         <f t="shared" si="5"/>
         <v>20.563949999999998</v>
       </c>
-      <c r="O10" s="20">
+      <c r="O10" s="4">
         <f t="shared" si="5"/>
         <v>58.349499999999999</v>
       </c>
-      <c r="P10" s="21">
+      <c r="P10" s="5">
         <f t="shared" si="6"/>
         <v>1.6282191104448664</v>
       </c>
-      <c r="Q10" s="21">
+      <c r="Q10" s="5">
         <f t="shared" si="6"/>
         <v>7.552946946074222</v>
       </c>
-      <c r="R10" s="22">
+      <c r="R10" s="17">
         <f>K10/2.205</f>
         <v>115.19274376417233</v>
       </c>
-      <c r="S10" s="35">
+      <c r="S10" s="27">
         <f>(C10*L10*1000/9.81)/D10</f>
         <v>0.94146564631413721</v>
       </c>
-      <c r="T10" s="21">
+      <c r="T10" s="5">
         <f>(C10*L10*1000/9.81)/F10</f>
         <v>0.67147961612737928</v>
       </c>
-      <c r="U10" s="21">
+      <c r="U10" s="5">
         <f>(C10*M10*1000/9.81)/D10</f>
         <v>1.5391376577382805</v>
       </c>
-      <c r="V10" s="21">
+      <c r="V10" s="5">
         <f>(C10*M10*1000/9.81)/F10</f>
         <v>1.0977560016464458</v>
       </c>
-      <c r="W10" s="21">
+      <c r="W10" s="5">
         <f>E10/(P10*C10)</f>
         <v>1965.3374533392421</v>
       </c>
-      <c r="X10" s="21">
+      <c r="X10" s="5">
         <f>E10/(Q10*C10)</f>
         <v>423.6756888201441</v>
       </c>
-      <c r="Y10" s="21">
+      <c r="Y10" s="5">
         <f>W10*0.33</f>
         <v>648.5613596019499</v>
       </c>
-      <c r="Z10" s="22">
+      <c r="Z10" s="17">
         <f>Q10/P10</f>
         <v>4.638777973813724</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11" s="8"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="20"/>
-      <c r="M11" s="20"/>
-      <c r="N11" s="20"/>
-      <c r="O11" s="20"/>
-      <c r="P11" s="21"/>
-      <c r="Q11" s="21"/>
-      <c r="R11" s="22"/>
-      <c r="S11" s="35"/>
-      <c r="T11" s="21"/>
-      <c r="U11" s="21"/>
-      <c r="V11" s="21"/>
-      <c r="W11" s="21"/>
-      <c r="X11" s="21"/>
-      <c r="Y11" s="21"/>
-      <c r="Z11" s="22"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="16"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="17"/>
+      <c r="S11" s="27"/>
+      <c r="Z11" s="17"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12">
         <v>2</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="2">
         <v>12701</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="2">
         <v>6103</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="9">
         <v>20185</v>
       </c>
-      <c r="G12" s="18">
+      <c r="G12" s="16">
         <v>14670</v>
       </c>
-      <c r="H12" s="10">
+      <c r="H12" s="2">
         <v>23830</v>
       </c>
-      <c r="I12" s="23">
+      <c r="I12" s="18">
         <v>0.73499999999999999</v>
       </c>
-      <c r="J12" s="19">
+      <c r="J12" s="3">
         <v>2.1</v>
       </c>
-      <c r="K12" s="11">
+      <c r="K12" s="9">
         <v>228</v>
       </c>
-      <c r="L12" s="20">
+      <c r="L12" s="4">
         <f t="shared" ref="L12:M15" si="8">G12/224.809</f>
         <v>65.255394579398512</v>
       </c>
-      <c r="M12" s="20">
+      <c r="M12" s="4">
         <f t="shared" si="8"/>
         <v>106.00109426224039</v>
       </c>
-      <c r="N12" s="20">
+      <c r="N12" s="4">
         <f t="shared" ref="N12:O15" si="9">I12*28.325</f>
         <v>20.818874999999998</v>
       </c>
-      <c r="O12" s="20">
+      <c r="O12" s="4">
         <f t="shared" si="9"/>
         <v>59.482500000000002</v>
       </c>
-      <c r="P12" s="21">
+      <c r="P12" s="5">
         <f t="shared" ref="P12:Q15" si="10">L12*N12/1000</f>
         <v>1.358543902824175</v>
       </c>
-      <c r="Q12" s="21">
+      <c r="Q12" s="5">
         <f t="shared" si="10"/>
         <v>6.3052100894537144</v>
       </c>
-      <c r="R12" s="22">
+      <c r="R12" s="17">
         <f>K12/2.205</f>
         <v>103.40136054421768</v>
       </c>
-      <c r="S12" s="35">
+      <c r="S12" s="27">
         <f>(C12*L12*1000/9.81)/D12</f>
         <v>1.0474649323589988</v>
       </c>
-      <c r="T12" s="21">
+      <c r="T12" s="5">
         <f>(C12*L12*1000/9.81)/F12</f>
         <v>0.65909596759433453</v>
       </c>
-      <c r="U12" s="21">
+      <c r="U12" s="5">
         <f>(C12*M12*1000/9.81)/D12</f>
         <v>1.701505749019423</v>
       </c>
-      <c r="V12" s="21">
+      <c r="V12" s="5">
         <f>(C12*M12*1000/9.81)/F12</f>
         <v>1.0706378260240621</v>
       </c>
-      <c r="W12" s="21">
+      <c r="W12" s="5">
         <f>E12/(P12*C12)</f>
         <v>2246.1548674698442</v>
       </c>
-      <c r="X12" s="21">
+      <c r="X12" s="5">
         <f>E12/(Q12*C12)</f>
         <v>483.96484125152807</v>
       </c>
-      <c r="Y12" s="21">
+      <c r="Y12" s="5">
         <f>W12*0.33</f>
         <v>741.23110626504865</v>
       </c>
-      <c r="Z12" s="22">
+      <c r="Z12" s="17">
         <f>Q12/P12</f>
         <v>4.641152984711268</v>
       </c>
@@ -9599,93 +9620,93 @@
       <c r="A13" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" t="s">
         <v>78</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13">
         <v>2</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="2">
         <v>14379</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="2">
         <v>10591</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="9">
         <v>23000</v>
       </c>
-      <c r="G13" s="18">
+      <c r="G13" s="16">
         <v>14670</v>
       </c>
-      <c r="H13" s="10">
+      <c r="H13" s="2">
         <v>23830</v>
       </c>
-      <c r="I13" s="23">
+      <c r="I13" s="18">
         <v>0.73499999999999999</v>
       </c>
-      <c r="J13" s="19">
+      <c r="J13" s="3">
         <v>2.1</v>
       </c>
-      <c r="K13" s="11">
+      <c r="K13" s="9">
         <v>228</v>
       </c>
-      <c r="L13" s="20">
+      <c r="L13" s="4">
         <f t="shared" si="8"/>
         <v>65.255394579398512</v>
       </c>
-      <c r="M13" s="20">
+      <c r="M13" s="4">
         <f t="shared" si="8"/>
         <v>106.00109426224039</v>
       </c>
-      <c r="N13" s="20">
+      <c r="N13" s="4">
         <f t="shared" si="9"/>
         <v>20.818874999999998</v>
       </c>
-      <c r="O13" s="20">
+      <c r="O13" s="4">
         <f t="shared" si="9"/>
         <v>59.482500000000002</v>
       </c>
-      <c r="P13" s="21">
+      <c r="P13" s="5">
         <f t="shared" si="10"/>
         <v>1.358543902824175</v>
       </c>
-      <c r="Q13" s="21">
+      <c r="Q13" s="5">
         <f t="shared" si="10"/>
         <v>6.3052100894537144</v>
       </c>
-      <c r="R13" s="22">
+      <c r="R13" s="17">
         <f>K13/2.205</f>
         <v>103.40136054421768</v>
       </c>
-      <c r="S13" s="35">
+      <c r="S13" s="27">
         <f>(C13*L13*1000/9.81)/D13</f>
         <v>0.92522790916556386</v>
       </c>
-      <c r="T13" s="21">
+      <c r="T13" s="5">
         <f>(C13*L13*1000/9.81)/F13</f>
         <v>0.5784283524300714</v>
       </c>
-      <c r="U13" s="21">
+      <c r="U13" s="5">
         <f>(C13*M13*1000/9.81)/D13</f>
         <v>1.5029434952566725</v>
       </c>
-      <c r="V13" s="21">
+      <c r="V13" s="5">
         <f>(C13*M13*1000/9.81)/F13</f>
         <v>0.9396010660128562</v>
       </c>
-      <c r="W13" s="21">
+      <c r="W13" s="5">
         <f>E13/(P13*C13)</f>
         <v>3897.9233493975294</v>
       </c>
-      <c r="X13" s="21">
+      <c r="X13" s="5">
         <f>E13/(Q13*C13)</f>
         <v>839.86099192117547</v>
       </c>
-      <c r="Y13" s="21">
+      <c r="Y13" s="5">
         <f>W13*0.33</f>
         <v>1286.3147053011849</v>
       </c>
-      <c r="Z13" s="22">
+      <c r="Z13" s="17">
         <f>Q13/P13</f>
         <v>4.641152984711268</v>
       </c>
@@ -9694,93 +9715,93 @@
       <c r="A14" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14">
         <v>2</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="2">
         <v>14379</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="2">
         <v>10591</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F14" s="9">
         <v>23000</v>
       </c>
-      <c r="G14" s="18">
+      <c r="G14" s="16">
         <v>17000</v>
       </c>
-      <c r="H14" s="10">
+      <c r="H14" s="2">
         <v>29000</v>
       </c>
-      <c r="I14" s="23">
+      <c r="I14" s="18">
         <v>0.745</v>
       </c>
-      <c r="J14" s="19">
+      <c r="J14" s="3">
         <v>1.9</v>
       </c>
-      <c r="K14" s="11">
+      <c r="K14" s="9">
         <v>270</v>
       </c>
-      <c r="L14" s="20">
+      <c r="L14" s="4">
         <f t="shared" si="8"/>
         <v>75.619748319684717</v>
       </c>
-      <c r="M14" s="20">
+      <c r="M14" s="4">
         <f t="shared" si="8"/>
         <v>128.99839419240334</v>
       </c>
-      <c r="N14" s="20">
+      <c r="N14" s="4">
         <f t="shared" si="9"/>
         <v>21.102125000000001</v>
       </c>
-      <c r="O14" s="20">
+      <c r="O14" s="4">
         <f t="shared" si="9"/>
         <v>53.817499999999995</v>
       </c>
-      <c r="P14" s="21">
+      <c r="P14" s="5">
         <f t="shared" si="10"/>
         <v>1.5957373815105271</v>
       </c>
-      <c r="Q14" s="21">
+      <c r="Q14" s="5">
         <f t="shared" si="10"/>
         <v>6.942371079449666</v>
       </c>
-      <c r="R14" s="22">
+      <c r="R14" s="17">
         <f>K14/2.205</f>
         <v>122.44897959183673</v>
       </c>
-      <c r="S14" s="35">
+      <c r="S14" s="27">
         <f>(C14*L14*1000/9.81)/D14</f>
         <v>1.0721795811734551</v>
       </c>
-      <c r="T14" s="21">
+      <c r="T14" s="5">
         <f>(C14*L14*1000/9.81)/F14</f>
         <v>0.67029870424752658</v>
       </c>
-      <c r="U14" s="21">
+      <c r="U14" s="5">
         <f>(C14*M14*1000/9.81)/D14</f>
         <v>1.8290122267076587</v>
       </c>
-      <c r="V14" s="21">
+      <c r="V14" s="5">
         <f>(C14*M14*1000/9.81)/F14</f>
         <v>1.1434507307751924</v>
       </c>
-      <c r="W14" s="21">
+      <c r="W14" s="5">
         <f>E14/(P14*C14)</f>
         <v>3318.5285131236774</v>
       </c>
-      <c r="X14" s="21">
+      <c r="X14" s="5">
         <f>E14/(Q14*C14)</f>
         <v>762.77973899657684</v>
       </c>
-      <c r="Y14" s="21">
+      <c r="Y14" s="5">
         <f>W14*0.33</f>
         <v>1095.1144093308135</v>
       </c>
-      <c r="Z14" s="22">
+      <c r="Z14" s="17">
         <f>Q14/P14</f>
         <v>4.3505724437425961</v>
       </c>
@@ -9789,216 +9810,202 @@
       <c r="A15" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15">
         <v>2</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="2">
         <v>14379</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E15" s="2">
         <v>10591</v>
       </c>
-      <c r="F15" s="11">
+      <c r="F15" s="9">
         <v>23000</v>
       </c>
-      <c r="G15" s="18">
+      <c r="G15" s="16">
         <v>17800</v>
       </c>
-      <c r="H15" s="10">
+      <c r="H15" s="2">
         <v>29100</v>
       </c>
-      <c r="I15" s="19">
+      <c r="I15" s="3">
         <v>0.72599999999999998</v>
       </c>
-      <c r="J15" s="19">
+      <c r="J15" s="3">
         <v>2.06</v>
       </c>
-      <c r="K15" s="11">
+      <c r="K15" s="9">
         <v>254</v>
       </c>
-      <c r="L15" s="20">
+      <c r="L15" s="4">
         <f t="shared" si="8"/>
         <v>79.178324711199281</v>
       </c>
-      <c r="M15" s="20">
+      <c r="M15" s="4">
         <f t="shared" si="8"/>
         <v>129.44321624134264</v>
       </c>
-      <c r="N15" s="20">
+      <c r="N15" s="4">
         <f t="shared" si="9"/>
         <v>20.563949999999998</v>
       </c>
-      <c r="O15" s="20">
+      <c r="O15" s="4">
         <f t="shared" si="9"/>
         <v>58.349499999999999</v>
       </c>
-      <c r="P15" s="21">
+      <c r="P15" s="5">
         <f t="shared" si="10"/>
         <v>1.6282191104448664</v>
       </c>
-      <c r="Q15" s="21">
+      <c r="Q15" s="5">
         <f t="shared" si="10"/>
         <v>7.552946946074222</v>
       </c>
-      <c r="R15" s="22">
+      <c r="R15" s="17">
         <f>K15/2.205</f>
         <v>115.19274376417233</v>
       </c>
-      <c r="S15" s="35">
+      <c r="S15" s="27">
         <f>(C15*L15*1000/9.81)/D15</f>
         <v>1.1226350908757352</v>
       </c>
-      <c r="T15" s="21">
+      <c r="T15" s="5">
         <f>(C15*L15*1000/9.81)/F15</f>
         <v>0.70184217268270421</v>
       </c>
-      <c r="U15" s="21">
+      <c r="U15" s="5">
         <f>(C15*M15*1000/9.81)/D15</f>
         <v>1.8353191654204435</v>
       </c>
-      <c r="V15" s="21">
+      <c r="V15" s="5">
         <f>(C15*M15*1000/9.81)/F15</f>
         <v>1.1473936643295894</v>
       </c>
-      <c r="W15" s="21">
+      <c r="W15" s="5">
         <f>E15/(P15*C15)</f>
         <v>3252.3264012993614</v>
       </c>
-      <c r="X15" s="21">
+      <c r="X15" s="5">
         <f>E15/(Q15*C15)</f>
         <v>701.11706567096041</v>
       </c>
-      <c r="Y15" s="21">
+      <c r="Y15" s="5">
         <f>W15*0.33</f>
         <v>1073.2677124287893</v>
       </c>
-      <c r="Z15" s="22">
+      <c r="Z15" s="17">
         <f>Q15/P15</f>
         <v>4.638777973813724</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16" s="8"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="19"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="20"/>
-      <c r="M16" s="20"/>
-      <c r="N16" s="20"/>
-      <c r="O16" s="20"/>
-      <c r="P16" s="21"/>
-      <c r="Q16" s="21"/>
-      <c r="R16" s="22"/>
-      <c r="S16" s="35"/>
-      <c r="T16" s="21"/>
-      <c r="U16" s="21"/>
-      <c r="V16" s="21"/>
-      <c r="W16" s="21"/>
-      <c r="X16" s="21"/>
-      <c r="Y16" s="21"/>
-      <c r="Z16" s="22"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="16"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="17"/>
+      <c r="S16" s="27"/>
+      <c r="Z16" s="17"/>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17">
         <v>2</v>
       </c>
-      <c r="D17" s="10">
+      <c r="D17" s="2">
         <v>19838</v>
       </c>
-      <c r="E17" s="10">
+      <c r="E17" s="2">
         <v>7350</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F17" s="9">
         <v>27669</v>
       </c>
-      <c r="G17" s="24">
+      <c r="G17" s="19">
         <v>13400</v>
       </c>
-      <c r="H17" s="10">
+      <c r="H17" s="2">
         <v>20900</v>
       </c>
-      <c r="I17" s="23">
+      <c r="I17" s="18">
         <v>0.66700000000000004</v>
       </c>
-      <c r="J17" s="23">
+      <c r="J17" s="18">
         <v>2.5</v>
       </c>
-      <c r="K17" s="37">
+      <c r="K17" s="29">
         <v>260</v>
       </c>
-      <c r="L17" s="20">
+      <c r="L17" s="4">
         <f>G17/224.809</f>
         <v>59.606154557869125</v>
       </c>
-      <c r="M17" s="20">
+      <c r="M17" s="4">
         <f>H17/224.809</f>
         <v>92.967808228318262</v>
       </c>
-      <c r="N17" s="20">
+      <c r="N17" s="4">
         <f>I17*28.325</f>
         <v>18.892775</v>
       </c>
-      <c r="O17" s="20">
+      <c r="O17" s="4">
         <f>J17*28.325</f>
         <v>70.8125</v>
       </c>
-      <c r="P17" s="21">
+      <c r="P17" s="5">
         <f>L17*N17/1000</f>
         <v>1.1261256666770461</v>
       </c>
-      <c r="Q17" s="21">
+      <c r="Q17" s="5">
         <f>M17*O17/1000</f>
         <v>6.5832829201677869</v>
       </c>
-      <c r="R17" s="22">
+      <c r="R17" s="17">
         <f>K17/2.205</f>
         <v>117.91383219954648</v>
       </c>
-      <c r="S17" s="35">
+      <c r="S17" s="27">
         <f>(C17*L17*1000/9.81)/D17</f>
         <v>0.61256786040186595</v>
       </c>
-      <c r="T17" s="21">
+      <c r="T17" s="5">
         <f>(C17*L17*1000/9.81)/F17</f>
         <v>0.43919625626702141</v>
       </c>
-      <c r="U17" s="21">
+      <c r="U17" s="5">
         <f>(C17*M17*1000/9.81)/D17</f>
         <v>0.95542300614917886</v>
       </c>
-      <c r="V17" s="21">
+      <c r="V17" s="5">
         <f>(C17*M17*1000/9.81)/F17</f>
         <v>0.68501505641647376</v>
       </c>
-      <c r="W17" s="21">
+      <c r="W17" s="5">
         <f>E17/(P17*C17)</f>
         <v>3263.4013314376648</v>
       </c>
-      <c r="X17" s="21">
+      <c r="X17" s="5">
         <f>E17/(Q17*C17)</f>
         <v>558.23212287317824</v>
       </c>
-      <c r="Y17" s="21">
+      <c r="Y17" s="5">
         <f t="shared" ref="Y17:Y18" si="11">W17*0.33</f>
         <v>1076.9224393744294</v>
       </c>
-      <c r="Z17" s="22">
+      <c r="Z17" s="17">
         <f>Q17/P17</f>
         <v>5.845957618205821</v>
       </c>
@@ -10007,432 +10014,389 @@
       <c r="A18" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18">
         <v>2</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D18" s="2">
         <v>19838</v>
       </c>
-      <c r="E18" s="10">
+      <c r="E18" s="2">
         <v>7350</v>
       </c>
-      <c r="F18" s="11">
+      <c r="F18" s="9">
         <v>27669</v>
       </c>
-      <c r="G18" s="18">
+      <c r="G18" s="16">
         <v>16800</v>
       </c>
-      <c r="H18" s="10">
+      <c r="H18" s="2">
         <v>26080</v>
       </c>
-      <c r="I18" s="23">
+      <c r="I18" s="18">
         <v>0.745</v>
       </c>
-      <c r="J18" s="19">
+      <c r="J18" s="3">
         <v>2</v>
       </c>
-      <c r="K18" s="11">
+      <c r="K18" s="9">
         <v>250</v>
       </c>
-      <c r="L18" s="20">
+      <c r="L18" s="4">
         <f>G18/224.809</f>
         <v>74.730104221806073</v>
       </c>
-      <c r="M18" s="20">
+      <c r="M18" s="4">
         <f>H18/224.809</f>
         <v>116.00959036337514</v>
       </c>
-      <c r="N18" s="20">
+      <c r="N18" s="4">
         <f>I18*28.325</f>
         <v>21.102125000000001</v>
       </c>
-      <c r="O18" s="20">
+      <c r="O18" s="4">
         <f>J18*28.325</f>
         <v>56.65</v>
       </c>
-      <c r="P18" s="21">
+      <c r="P18" s="5">
         <f>L18*N18/1000</f>
         <v>1.5769640005515797</v>
       </c>
-      <c r="Q18" s="21">
+      <c r="Q18" s="5">
         <f>M18*O18/1000</f>
         <v>6.5719432940852007</v>
       </c>
-      <c r="R18" s="22">
+      <c r="R18" s="17">
         <f>K18/2.205</f>
         <v>113.37868480725623</v>
       </c>
-      <c r="S18" s="35">
+      <c r="S18" s="27">
         <f>(C18*L18*1000/9.81)/D18</f>
         <v>0.76799552647398128</v>
       </c>
-      <c r="T18" s="21">
+      <c r="T18" s="5">
         <f>(C18*L18*1000/9.81)/F18</f>
         <v>0.55063411233477322</v>
       </c>
-      <c r="U18" s="21">
+      <c r="U18" s="5">
         <f>(C18*M18*1000/9.81)/D18</f>
         <v>1.1922216268119898</v>
       </c>
-      <c r="V18" s="21">
+      <c r="V18" s="5">
         <f>(C18*M18*1000/9.81)/F18</f>
         <v>0.85479390771969554</v>
       </c>
-      <c r="W18" s="21">
+      <c r="W18" s="5">
         <f>E18/(P18*C18)</f>
         <v>2330.4273266317959</v>
       </c>
-      <c r="X18" s="21">
+      <c r="X18" s="5">
         <f>E18/(Q18*C18)</f>
         <v>559.19533014040587</v>
       </c>
-      <c r="Y18" s="21">
+      <c r="Y18" s="5">
         <f t="shared" si="11"/>
         <v>769.0410177884927</v>
       </c>
-      <c r="Z18" s="22">
+      <c r="Z18" s="17">
         <f>Q18/P18</f>
         <v>4.1674656439757101</v>
       </c>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A19" s="8"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="19"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="20"/>
-      <c r="M19" s="20"/>
-      <c r="N19" s="20"/>
-      <c r="O19" s="20"/>
-      <c r="P19" s="21"/>
-      <c r="Q19" s="21"/>
-      <c r="R19" s="22"/>
-      <c r="S19" s="35"/>
-      <c r="T19" s="21"/>
-      <c r="U19" s="21"/>
-      <c r="V19" s="21"/>
-      <c r="W19" s="21"/>
-      <c r="X19" s="21"/>
-      <c r="Y19" s="21"/>
-      <c r="Z19" s="22"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="16"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="17"/>
+      <c r="S19" s="27"/>
+      <c r="Z19" s="17"/>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20">
         <v>2</v>
       </c>
-      <c r="D20" s="10">
+      <c r="D20" s="2">
         <v>11321</v>
       </c>
-      <c r="E20" s="10">
+      <c r="E20" s="2">
         <v>4990</v>
       </c>
-      <c r="F20" s="11">
+      <c r="F20" s="9">
         <v>13782</v>
       </c>
-      <c r="G20" s="18">
-        <v>9065</v>
-      </c>
-      <c r="H20" s="10"/>
-      <c r="I20" s="23">
+      <c r="G20" s="16">
+        <v>18130</v>
+      </c>
+      <c r="I20" s="18">
         <v>0.37</v>
       </c>
-      <c r="J20" s="19"/>
-      <c r="K20" s="11">
+      <c r="J20" s="3"/>
+      <c r="K20" s="9">
         <v>333</v>
       </c>
-      <c r="L20" s="20">
+      <c r="L20" s="4">
         <f>G20/224.809</f>
-        <v>40.323118736349521</v>
-      </c>
-      <c r="M20" s="20"/>
-      <c r="N20" s="20">
+        <v>80.646237472699042</v>
+      </c>
+      <c r="N20" s="4">
         <f>I20*28.325</f>
         <v>10.48025</v>
       </c>
-      <c r="O20" s="20"/>
-      <c r="P20" s="21">
+      <c r="O20" s="4"/>
+      <c r="P20" s="5">
         <f>L20*N20/1000</f>
-        <v>0.42259636513662707</v>
-      </c>
-      <c r="Q20" s="21"/>
-      <c r="R20" s="22">
+        <v>0.84519273027325414</v>
+      </c>
+      <c r="Q20" s="5"/>
+      <c r="R20" s="17">
         <f>K20/2.205</f>
         <v>151.0204081632653</v>
       </c>
-      <c r="S20" s="35">
+      <c r="S20" s="27">
         <f>(C20*L20*1000/9.81)/D20</f>
-        <v>0.7261566393640555</v>
-      </c>
-      <c r="T20" s="21">
+        <v>1.452313278728111</v>
+      </c>
+      <c r="T20" s="5">
         <f>(C20*L20*1000/9.81)/F20</f>
-        <v>0.59648957438981809</v>
-      </c>
-      <c r="U20" s="21"/>
-      <c r="V20" s="21"/>
-      <c r="W20" s="21">
+        <v>1.1929791487796362</v>
+      </c>
+      <c r="W20" s="5">
         <f>E20/(P20*C20)</f>
-        <v>5903.9788456139622</v>
-      </c>
-      <c r="X20" s="21"/>
-      <c r="Y20" s="21">
+        <v>2951.9894228069811</v>
+      </c>
+      <c r="Y20" s="5">
         <f t="shared" ref="Y20" si="12">W20*0.33</f>
-        <v>1948.3130190526076</v>
-      </c>
-      <c r="Z20" s="22"/>
+        <v>974.15650952630381</v>
+      </c>
+      <c r="Z20" s="17"/>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A21" s="8"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="19"/>
-      <c r="J21" s="19"/>
-      <c r="K21" s="11"/>
-      <c r="L21" s="20"/>
-      <c r="M21" s="20"/>
-      <c r="N21" s="20"/>
-      <c r="O21" s="20"/>
-      <c r="P21" s="21"/>
-      <c r="Q21" s="21"/>
-      <c r="R21" s="22"/>
-      <c r="S21" s="35"/>
-      <c r="T21" s="21"/>
-      <c r="U21" s="21"/>
-      <c r="V21" s="21"/>
-      <c r="W21" s="21"/>
-      <c r="X21" s="21"/>
-      <c r="Y21" s="21"/>
-      <c r="Z21" s="22"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="16"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="Q21" s="5"/>
+      <c r="R21" s="17"/>
+      <c r="S21" s="27"/>
+      <c r="Z21" s="17"/>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="9">
+      <c r="C22">
         <v>1</v>
       </c>
-      <c r="D22" s="12">
+      <c r="D22" s="10">
         <v>6340</v>
       </c>
-      <c r="E22" s="12">
+      <c r="E22" s="10">
         <v>3400</v>
       </c>
-      <c r="F22" s="13">
+      <c r="F22" s="11">
         <v>10410</v>
       </c>
-      <c r="G22" s="18">
+      <c r="G22" s="16">
         <v>21450</v>
       </c>
-      <c r="H22" s="10"/>
-      <c r="I22" s="19">
+      <c r="I22" s="3">
         <v>0.74</v>
       </c>
-      <c r="J22" s="19"/>
-      <c r="K22" s="37">
+      <c r="J22" s="3"/>
+      <c r="K22" s="29">
         <v>459</v>
       </c>
-      <c r="L22" s="20">
+      <c r="L22" s="4">
         <f>G22/224.809</f>
         <v>95.41432949748453</v>
       </c>
-      <c r="M22" s="20"/>
-      <c r="N22" s="20">
+      <c r="N22" s="4">
         <f>I22*28.325</f>
         <v>20.9605</v>
       </c>
-      <c r="O22" s="20"/>
-      <c r="P22" s="21">
+      <c r="O22" s="4"/>
+      <c r="P22" s="5">
         <f>L22*N22/1000</f>
         <v>1.9999320534320246</v>
       </c>
-      <c r="Q22" s="21"/>
-      <c r="R22" s="22">
+      <c r="Q22" s="5"/>
+      <c r="R22" s="17">
         <f>K22/2.205</f>
         <v>208.16326530612244</v>
       </c>
-      <c r="S22" s="35">
+      <c r="S22" s="27">
         <f>(C22*L22*1000/9.81)/D22</f>
         <v>1.5341058904273392</v>
       </c>
-      <c r="T22" s="21">
+      <c r="T22" s="5">
         <f>(C22*L22*1000/9.81)/F22</f>
         <v>0.93431617149945534</v>
       </c>
-      <c r="U22" s="21"/>
-      <c r="V22" s="21"/>
-      <c r="W22" s="21">
+      <c r="W22" s="5">
         <f>E22/(P22*C22)</f>
         <v>1700.0577565449585</v>
       </c>
-      <c r="X22" s="21"/>
-      <c r="Y22" s="21">
+      <c r="Y22" s="5">
         <f t="shared" ref="Y22:Y24" si="13">W22*0.33</f>
         <v>561.01905965983633</v>
       </c>
-      <c r="Z22" s="22"/>
+      <c r="Z22" s="17"/>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B23" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="9">
+      <c r="C23">
         <v>1</v>
       </c>
-      <c r="D23" s="12">
+      <c r="D23" s="10">
         <v>6340</v>
       </c>
-      <c r="E23" s="12">
+      <c r="E23" s="10">
         <v>3400</v>
       </c>
-      <c r="F23" s="13">
+      <c r="F23" s="11">
         <v>10410</v>
       </c>
-      <c r="G23" s="18">
+      <c r="G23" s="16">
         <v>23800</v>
       </c>
-      <c r="H23" s="10"/>
-      <c r="I23" s="19">
+      <c r="I23" s="3">
         <v>0.76</v>
       </c>
-      <c r="J23" s="19"/>
-      <c r="K23" s="11">
+      <c r="J23" s="3"/>
+      <c r="K23" s="9">
         <v>459</v>
       </c>
-      <c r="L23" s="20">
+      <c r="L23" s="4">
         <f>G23/224.809</f>
         <v>105.8676476475586</v>
       </c>
-      <c r="M23" s="20"/>
-      <c r="N23" s="20">
+      <c r="N23" s="4">
         <f>I23*28.325</f>
         <v>21.527000000000001</v>
       </c>
-      <c r="O23" s="20"/>
-      <c r="P23" s="21">
+      <c r="O23" s="4"/>
+      <c r="P23" s="5">
         <f>L23*N23/1000</f>
         <v>2.2790128509089942</v>
       </c>
-      <c r="Q23" s="21"/>
-      <c r="R23" s="22">
+      <c r="Q23" s="5"/>
+      <c r="R23" s="17">
         <f>K23/2.205</f>
         <v>208.16326530612244</v>
       </c>
-      <c r="S23" s="35">
+      <c r="S23" s="27">
         <f>(C23*L23*1000/9.81)/D23</f>
         <v>1.7021780975370941</v>
       </c>
-      <c r="T23" s="21">
+      <c r="T23" s="5">
         <f>(C23*L23*1000/9.81)/F23</f>
         <v>1.0366771506614003</v>
       </c>
-      <c r="U23" s="21"/>
-      <c r="V23" s="21"/>
-      <c r="W23" s="21">
+      <c r="W23" s="5">
         <f>E23/(P23*C23)</f>
         <v>1491.873992129485</v>
       </c>
-      <c r="X23" s="21"/>
-      <c r="Y23" s="21">
+      <c r="Y23" s="5">
         <f t="shared" si="13"/>
         <v>492.31841740273006</v>
       </c>
-      <c r="Z23" s="22"/>
+      <c r="Z23" s="17"/>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A24" s="14" t="s">
+      <c r="A24" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C24" s="15">
+      <c r="C24" s="13">
         <v>1</v>
       </c>
-      <c r="D24" s="16">
+      <c r="D24" s="14">
         <v>6340</v>
       </c>
-      <c r="E24" s="16">
+      <c r="E24" s="14">
         <v>3400</v>
       </c>
-      <c r="F24" s="17">
+      <c r="F24" s="15">
         <v>10410</v>
       </c>
-      <c r="G24" s="25">
+      <c r="G24" s="20">
         <v>23800</v>
       </c>
-      <c r="H24" s="26"/>
-      <c r="I24" s="27">
+      <c r="H24" s="21"/>
+      <c r="I24" s="22">
         <v>0.6</v>
       </c>
-      <c r="J24" s="28"/>
-      <c r="K24" s="38">
+      <c r="J24" s="23"/>
+      <c r="K24" s="30">
         <v>450</v>
       </c>
-      <c r="L24" s="29">
+      <c r="L24" s="24">
         <f>G24/224.809</f>
         <v>105.8676476475586</v>
       </c>
-      <c r="M24" s="29"/>
-      <c r="N24" s="29">
+      <c r="M24" s="24"/>
+      <c r="N24" s="24">
         <f>I24*28.325</f>
         <v>16.994999999999997</v>
       </c>
-      <c r="O24" s="29"/>
-      <c r="P24" s="30">
+      <c r="O24" s="24"/>
+      <c r="P24" s="25">
         <f>L24*N24/1000</f>
         <v>1.7992206717702581</v>
       </c>
-      <c r="Q24" s="30"/>
-      <c r="R24" s="31">
+      <c r="Q24" s="25"/>
+      <c r="R24" s="26">
         <f>K24/2.205</f>
         <v>204.08163265306121</v>
       </c>
-      <c r="S24" s="36">
+      <c r="S24" s="28">
         <f>(C24*L24*1000/9.81)/D24</f>
         <v>1.7021780975370941</v>
       </c>
-      <c r="T24" s="30">
+      <c r="T24" s="25">
         <f>(C24*L24*1000/9.81)/F24</f>
         <v>1.0366771506614003</v>
       </c>
-      <c r="U24" s="30"/>
-      <c r="V24" s="30"/>
-      <c r="W24" s="30">
+      <c r="U24" s="25"/>
+      <c r="V24" s="25"/>
+      <c r="W24" s="25">
         <f>E24/(P24*C24)</f>
         <v>1889.7070566973482</v>
       </c>
-      <c r="X24" s="30"/>
-      <c r="Y24" s="30">
+      <c r="X24" s="25"/>
+      <c r="Y24" s="25">
         <f t="shared" si="13"/>
         <v>623.60332871012497</v>
       </c>
-      <c r="Z24" s="31"/>
+      <c r="Z24" s="26"/>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
@@ -10463,14 +10427,17 @@
     <hyperlink ref="G31" r:id="rId1" xr:uid="{48D92612-8370-4284-8298-A8CA906B3BF7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA9BA4F5-4601-45D4-A8D5-481C1BEBEC64}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA9BA4F5-4601-45D4-A8D5-481C1BEBEC64}">
   <dimension ref="A1:S117"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -10550,7 +10517,7 @@
       </c>
       <c r="D2" s="1">
         <f>IRL!$T$20</f>
-        <v>0.59648957438981809</v>
+        <v>1.1929791487796362</v>
       </c>
       <c r="F2" t="s">
         <v>40</v>
@@ -10648,7 +10615,7 @@
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4">
         <f>IRL!$L$20*1000</f>
-        <v>40323.118736349519</v>
+        <v>80646.237472699038</v>
       </c>
       <c r="B4">
         <f>IRL!$R$20</f>
@@ -10656,10 +10623,10 @@
       </c>
       <c r="C4">
         <f>IRL!$P$20</f>
-        <v>0.42259636513662707</v>
+        <v>0.84519273027325414</v>
       </c>
       <c r="D4">
-        <v>1000</v>
+        <v>1200</v>
       </c>
       <c r="F4">
         <f>IRL!$L$22*1000</f>
@@ -10763,7 +10730,7 @@
       </c>
       <c r="B7">
         <f>D7/SQRT(B$2)/0.152</f>
-        <v>1.2173859264207616</v>
+        <v>2.4347718528415232</v>
       </c>
       <c r="C7">
         <f t="shared" ref="C7:C27" si="0">(1+(A7/1225)^2)*MAX(1-A7/D$4, 0)</f>
@@ -10771,7 +10738,7 @@
       </c>
       <c r="D7">
         <f>D2*9.81</f>
-        <v>5.8515627247641158</v>
+        <v>11.703125449528232</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -10826,15 +10793,15 @@
       </c>
       <c r="B8">
         <f t="shared" ref="B8:B27" si="8">D8/SQRT(B$2)/0.152</f>
-        <v>1.1303030306012005</v>
+        <v>2.2911547917591899</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>0.92846730528946264</v>
+        <v>0.94101416076634725</v>
       </c>
       <c r="D8">
         <f t="shared" ref="D8:D27" si="9">D$7*C8</f>
-        <v>5.432984674794004</v>
+        <v>11.012806773231089</v>
       </c>
       <c r="F8">
         <f t="shared" ref="F8:F27" si="10">F7+H$2</f>
@@ -10892,15 +10859,15 @@
       </c>
       <c r="B9">
         <f t="shared" si="8"/>
-        <v>1.05029324335039</v>
+        <v>2.1623684421919798</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>0.86274468971261975</v>
+        <v>0.88811953352769679</v>
       </c>
       <c r="D9">
         <f t="shared" si="9"/>
-        <v>5.0484046673105487</v>
+        <v>10.393774315051131</v>
       </c>
       <c r="F9">
         <f t="shared" si="10"/>
@@ -10958,15 +10925,15 @@
       </c>
       <c r="B10">
         <f t="shared" si="8"/>
-        <v>0.97530308153546696</v>
+        <v>2.0449903322517855</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>0.80114535610162441</v>
+        <v>0.83991045397750941</v>
       </c>
       <c r="D10">
         <f t="shared" si="9"/>
-        <v>4.687952302882139</v>
+        <v>9.8295774092690014</v>
       </c>
       <c r="F10">
         <f t="shared" si="10"/>
@@ -11024,15 +10991,15 @@
       </c>
       <c r="B11">
         <f t="shared" si="8"/>
-        <v>0.90327906202356789</v>
+        <v>1.9355979900505027</v>
       </c>
       <c r="C11">
         <f>(1+(A11/1225)^2)*MAX(1-A11/D$4, 0)</f>
-        <v>0.74198250728862969</v>
+        <v>0.79498125780924611</v>
       </c>
       <c r="D11">
         <f t="shared" si="9"/>
-        <v>4.3417571820771643</v>
+        <v>9.3037653901653528</v>
       </c>
       <c r="F11">
         <f t="shared" si="10"/>
@@ -11090,15 +11057,15 @@
       </c>
       <c r="B12">
         <f t="shared" si="8"/>
-        <v>0.83216770168183041</v>
+        <v>1.830768943700027</v>
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>0.68356934610578923</v>
+        <v>0.75192628071636824</v>
       </c>
       <c r="D12">
         <f t="shared" si="9"/>
-        <v>3.9999489054640169</v>
+        <v>8.7998875920208377</v>
       </c>
       <c r="F12">
         <f t="shared" si="10"/>
@@ -11156,15 +11123,15 @@
       </c>
       <c r="B13">
         <f t="shared" si="8"/>
-        <v>0.75991551737739138</v>
+        <v>1.7270807213122525</v>
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>0.62421907538525623</v>
+        <v>0.7093398583923366</v>
       </c>
       <c r="D13">
         <f t="shared" si="9"/>
-        <v>3.652657073611087</v>
+        <v>8.3014933491161056</v>
       </c>
       <c r="F13">
         <f t="shared" si="10"/>
@@ -11222,15 +11189,15 @@
       </c>
       <c r="B14">
         <f t="shared" si="8"/>
-        <v>0.68446902597738735</v>
+        <v>1.6211108509990753</v>
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
-        <v>0.56224489795918364</v>
+        <v>0.66581632653061229</v>
       </c>
       <c r="D14">
         <f t="shared" si="9"/>
-        <v>3.290011287086763</v>
+        <v>7.7921319957318076</v>
       </c>
       <c r="F14">
         <f t="shared" si="10"/>
@@ -11288,15 +11255,15 @@
       </c>
       <c r="B15">
         <f t="shared" si="8"/>
-        <v>0.60377474434895584</v>
+        <v>1.5094368608723896</v>
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
-        <v>0.49596001665972517</v>
+        <v>0.61995002082465644</v>
       </c>
       <c r="D15">
         <f t="shared" si="9"/>
-        <v>2.9021411464594378</v>
+        <v>7.255352866148594</v>
       </c>
       <c r="F15">
         <f t="shared" si="10"/>
@@ -11354,15 +11321,15 @@
       </c>
       <c r="B16">
         <f t="shared" si="8"/>
-        <v>0.5157791893592335</v>
+        <v>1.3886362790440903</v>
       </c>
       <c r="C16">
         <f t="shared" si="0"/>
-        <v>0.42367763431903371</v>
+        <v>0.57033527696793007</v>
       </c>
       <c r="D16">
         <f t="shared" si="9"/>
-        <v>2.4791762522974996</v>
+        <v>6.674705294647115</v>
       </c>
       <c r="F16">
         <f t="shared" si="10"/>
@@ -11420,15 +11387,15 @@
       </c>
       <c r="B17">
         <f t="shared" si="8"/>
-        <v>0.41842887787535749</v>
+        <v>1.2552866336260726</v>
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>0.34371095376926281</v>
+        <v>0.51556643065389418</v>
       </c>
       <c r="D17">
         <f t="shared" si="9"/>
-        <v>2.0112462051693405</v>
+        <v>6.033738615508021</v>
       </c>
       <c r="F17">
         <f t="shared" si="10"/>
@@ -11486,15 +11453,15 @@
       </c>
       <c r="B18">
         <f t="shared" si="8"/>
-        <v>0.30967032676446493</v>
+        <v>1.1059654527302316</v>
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>0.25437317784256563</v>
+        <v>0.45423781757601001</v>
       </c>
       <c r="D18">
         <f t="shared" si="9"/>
-        <v>1.4884806056433504</v>
+        <v>5.3160021630119649</v>
       </c>
       <c r="F18">
         <f t="shared" si="10"/>
@@ -11552,15 +11519,15 @@
       </c>
       <c r="B19">
         <f t="shared" si="8"/>
-        <v>0.18745005289369238</v>
+        <v>0.93725026446846216</v>
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>0.15397750937109533</v>
+        <v>0.38494377342773844</v>
       </c>
       <c r="D19">
         <f t="shared" si="9"/>
-        <v>0.90100905428791878</v>
+        <v>4.5050452714395952</v>
       </c>
       <c r="F19">
         <f t="shared" si="10"/>
@@ -11618,15 +11585,15 @@
       </c>
       <c r="B20">
         <f t="shared" si="8"/>
-        <v>4.9714573130177332E-2</v>
+        <v>0.74571859695265941</v>
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>4.0837151187005455E-2</v>
+        <v>0.30627863390254062</v>
       </c>
       <c r="D20">
         <f t="shared" si="9"/>
-        <v>0.23896115167143778</v>
+        <v>3.5844172750715635</v>
       </c>
       <c r="F20">
         <f t="shared" si="10"/>
@@ -11684,15 +11651,15 @@
       </c>
       <c r="B21">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>0.52794797829471796</v>
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.21683673469387754</v>
       </c>
       <c r="D21">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>2.5376675081885196</v>
       </c>
       <c r="F21">
         <f t="shared" si="10"/>
@@ -11750,15 +11717,15 @@
       </c>
       <c r="B22">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>0.28051593660653323</v>
       </c>
       <c r="C22">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.11521241149521033</v>
       </c>
       <c r="D22">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1.3483453050711149</v>
       </c>
       <c r="F22">
         <f t="shared" si="10"/>
@@ -16698,6 +16665,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>